<commit_message>
Issue #17: Adds ESEM into the venues of interest
</commit_message>
<xml_diff>
--- a/resources/filtered_papers.xlsx
+++ b/resources/filtered_papers.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H256"/>
+  <dimension ref="A1:H261"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7755,10 +7755,235 @@
     <row r="178">
       <c r="A178" t="inlineStr">
         <is>
+          <t>Paul Luo Li and Randy Nakagawa and Rob Montroy</t>
+        </is>
+      </c>
+      <c r="B178" t="inlineStr">
+        <is>
+          <t>@inproceedings{luo:2007,
+booktitle = {International Symposium on Empirical Software Engineering and Measurement (ESEM)}, 
+author = {Paul Luo Li and Randy Nakagawa and Rob Montroy}, 
+title = {{Estimating the Quality of Widely Used Software Products Using Software Reliability Growth Modeling: Case Study of an IBM Federated Database Project}}, 
+year = {2007} 
+}</t>
+        </is>
+      </c>
+      <c r="C178" t="inlineStr">
+        <is>
+          <t>conf/esem/LiNM07</t>
+        </is>
+      </c>
+      <c r="D178" t="inlineStr">
+        <is>
+          <t>Estimating the Quality of Widely Used Software Products Using Software Reliability Growth Modeling: Case Study of an IBM Federated Database Project</t>
+        </is>
+      </c>
+      <c r="E178" t="inlineStr">
+        <is>
+          <t>db/conf/esem/esem2007.html#LiNM07</t>
+        </is>
+      </c>
+      <c r="F178" t="inlineStr">
+        <is>
+          <t>conf/esem/</t>
+        </is>
+      </c>
+      <c r="G178" t="n">
+        <v>2007</v>
+      </c>
+      <c r="H178" t="inlineStr">
+        <is>
+          <t>conf/esem/2007</t>
+        </is>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" t="inlineStr">
+        <is>
+          <t>Donald W. McCormick II and William B. Frakes and Reghu Anguswamy</t>
+        </is>
+      </c>
+      <c r="B179" t="inlineStr">
+        <is>
+          <t>@inproceedings{w.:2012,
+booktitle = {International Symposium on Empirical Software Engineering and Measurement (ESEM)}, 
+author = {Donald W. McCormick II and William B. Frakes and Reghu Anguswamy}, 
+title = {{A comparison of database fault detection capabilities using mutation testing}}, 
+year = {2012} 
+}</t>
+        </is>
+      </c>
+      <c r="C179" t="inlineStr">
+        <is>
+          <t>conf/esem/McCormickFA12</t>
+        </is>
+      </c>
+      <c r="D179" t="inlineStr">
+        <is>
+          <t>A comparison of database fault detection capabilities using mutation testing</t>
+        </is>
+      </c>
+      <c r="E179" t="inlineStr">
+        <is>
+          <t>db/conf/esem/esem2012.html#McCormickFA12</t>
+        </is>
+      </c>
+      <c r="F179" t="inlineStr">
+        <is>
+          <t>conf/esem/</t>
+        </is>
+      </c>
+      <c r="G179" t="n">
+        <v>2012</v>
+      </c>
+      <c r="H179" t="inlineStr">
+        <is>
+          <t>conf/esem/2012</t>
+        </is>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" t="inlineStr">
+        <is>
+          <t>Rudolf Ramler and Klaus Wolfmaier</t>
+        </is>
+      </c>
+      <c r="B180" t="inlineStr">
+        <is>
+          <t>@inproceedings{ramler:2008,
+booktitle = {International Symposium on Empirical Software Engineering and Measurement (ESEM)}, 
+author = {Rudolf Ramler and Klaus Wolfmaier}, 
+title = {{Issues and effort in integrating data from heterogeneous software repositories and corporate databases}}, 
+year = {2008} 
+}</t>
+        </is>
+      </c>
+      <c r="C180" t="inlineStr">
+        <is>
+          <t>conf/esem/RamlerW08</t>
+        </is>
+      </c>
+      <c r="D180" t="inlineStr">
+        <is>
+          <t>Issues and effort in integrating data from heterogeneous software repositories and corporate databases</t>
+        </is>
+      </c>
+      <c r="E180" t="inlineStr">
+        <is>
+          <t>db/conf/esem/esem2008.html#RamlerW08</t>
+        </is>
+      </c>
+      <c r="F180" t="inlineStr">
+        <is>
+          <t>conf/esem/</t>
+        </is>
+      </c>
+      <c r="G180" t="n">
+        <v>2008</v>
+      </c>
+      <c r="H180" t="inlineStr">
+        <is>
+          <t>conf/esem/2008</t>
+        </is>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" t="inlineStr">
+        <is>
+          <t>Michael Wedel and Uwe Jensen and Peter Göhner</t>
+        </is>
+      </c>
+      <c r="B181" t="inlineStr">
+        <is>
+          <t>@inproceedings{wedel:2008,
+booktitle = {International Symposium on Empirical Software Engineering and Measurement (ESEM)}, 
+author = {Michael Wedel and Uwe Jensen and Peter Göhner}, 
+title = {{Mining software code repositories and bug databases using survival analysis models}}, 
+year = {2008} 
+}</t>
+        </is>
+      </c>
+      <c r="C181" t="inlineStr">
+        <is>
+          <t>conf/esem/WedelJG08</t>
+        </is>
+      </c>
+      <c r="D181" t="inlineStr">
+        <is>
+          <t>Mining software code repositories and bug databases using survival analysis models</t>
+        </is>
+      </c>
+      <c r="E181" t="inlineStr">
+        <is>
+          <t>db/conf/esem/esem2008.html#WedelJG08</t>
+        </is>
+      </c>
+      <c r="F181" t="inlineStr">
+        <is>
+          <t>conf/esem/</t>
+        </is>
+      </c>
+      <c r="G181" t="n">
+        <v>2008</v>
+      </c>
+      <c r="H181" t="inlineStr">
+        <is>
+          <t>conf/esem/2008</t>
+        </is>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" t="inlineStr">
+        <is>
+          <t>Samireh Jalali and Claes Wohlin</t>
+        </is>
+      </c>
+      <c r="B182" t="inlineStr">
+        <is>
+          <t>@inproceedings{jalali:2012,
+booktitle = {International Symposium on Empirical Software Engineering and Measurement (ESEM)}, 
+author = {Samireh Jalali and Claes Wohlin}, 
+title = {{Systematic literature studies: database searches vs. backward snowballing}}, 
+year = {2012} 
+}</t>
+        </is>
+      </c>
+      <c r="C182" t="inlineStr">
+        <is>
+          <t>conf/esem/JalaliW12</t>
+        </is>
+      </c>
+      <c r="D182" t="inlineStr">
+        <is>
+          <t>Systematic literature studies: database searches vs. backward snowballing</t>
+        </is>
+      </c>
+      <c r="E182" t="inlineStr">
+        <is>
+          <t>db/conf/esem/esem2012.html#JalaliW12</t>
+        </is>
+      </c>
+      <c r="F182" t="inlineStr">
+        <is>
+          <t>conf/esem/</t>
+        </is>
+      </c>
+      <c r="G182" t="n">
+        <v>2012</v>
+      </c>
+      <c r="H182" t="inlineStr">
+        <is>
+          <t>conf/esem/2012</t>
+        </is>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" t="inlineStr">
+        <is>
           <t>Julien Delplanque</t>
         </is>
       </c>
-      <c r="B178" t="inlineStr">
+      <c r="B183" t="inlineStr">
         <is>
           <t>@inproceedings{delplanque:2018,
 booktitle = {International Conference on Automated Software Engineering(ASE)}, 
@@ -7768,42 +7993,42 @@
 }</t>
         </is>
       </c>
-      <c r="C178" t="inlineStr">
+      <c r="C183" t="inlineStr">
         <is>
           <t>conf/kbse/Delplanque18</t>
         </is>
       </c>
-      <c r="D178" t="inlineStr">
+      <c r="D183" t="inlineStr">
         <is>
           <t>Software engineering techniques applied to relational databases</t>
         </is>
       </c>
-      <c r="E178" t="inlineStr">
+      <c r="E183" t="inlineStr">
         <is>
           <t>db/conf/kbse/ase2018.html#Delplanque18</t>
         </is>
       </c>
-      <c r="F178" t="inlineStr">
+      <c r="F183" t="inlineStr">
         <is>
           <t>conf/kbse/</t>
         </is>
       </c>
-      <c r="G178" t="n">
+      <c r="G183" t="n">
         <v>2018</v>
       </c>
-      <c r="H178" t="inlineStr">
+      <c r="H183" t="inlineStr">
         <is>
           <t>conf/kbse/2018</t>
         </is>
       </c>
     </row>
-    <row r="179">
-      <c r="A179" t="inlineStr">
+    <row r="184">
+      <c r="A184" t="inlineStr">
         <is>
           <t>Yossi Cohen and Yishai A. Feldman</t>
         </is>
       </c>
-      <c r="B179" t="inlineStr">
+      <c r="B184" t="inlineStr">
         <is>
           <t>@inproceedings{cohen:1997,
 booktitle = {International Conference on Automated Software Engineering(ASE)}, 
@@ -7813,42 +8038,42 @@
 }</t>
         </is>
       </c>
-      <c r="C179" t="inlineStr">
+      <c r="C184" t="inlineStr">
         <is>
           <t>conf/kbse/CohenF97</t>
         </is>
       </c>
-      <c r="D179" t="inlineStr">
+      <c r="D184" t="inlineStr">
         <is>
           <t>Automatic High-Quality Reengineering of Database Programs by Temporal Abstraction</t>
         </is>
       </c>
-      <c r="E179" t="inlineStr">
+      <c r="E184" t="inlineStr">
         <is>
           <t>db/conf/kbse/ase1997.html#CohenF97</t>
         </is>
       </c>
-      <c r="F179" t="inlineStr">
+      <c r="F184" t="inlineStr">
         <is>
           <t>conf/kbse/</t>
         </is>
       </c>
-      <c r="G179" t="n">
+      <c r="G184" t="n">
         <v>1997</v>
       </c>
-      <c r="H179" t="inlineStr">
+      <c r="H184" t="inlineStr">
         <is>
           <t>conf/kbse/1997</t>
         </is>
       </c>
     </row>
-    <row r="180">
-      <c r="A180" t="inlineStr">
+    <row r="185">
+      <c r="A185" t="inlineStr">
         <is>
           <t>Shadi Abdul Khalek and Sarfraz Khurshid</t>
         </is>
       </c>
-      <c r="B180" t="inlineStr">
+      <c r="B185" t="inlineStr">
         <is>
           <t>@inproceedings{abdul:2010,
 booktitle = {International Conference on Automated Software Engineering(ASE)}, 
@@ -7858,42 +8083,42 @@
 }</t>
         </is>
       </c>
-      <c r="C180" t="inlineStr">
+      <c r="C185" t="inlineStr">
         <is>
           <t>conf/kbse/KhalekK10</t>
         </is>
       </c>
-      <c r="D180" t="inlineStr">
+      <c r="D185" t="inlineStr">
         <is>
           <t>Automated SQL query generation for systematic testing of database engines</t>
         </is>
       </c>
-      <c r="E180" t="inlineStr">
+      <c r="E185" t="inlineStr">
         <is>
           <t>db/conf/kbse/ase2010.html#KhalekK10</t>
         </is>
       </c>
-      <c r="F180" t="inlineStr">
+      <c r="F185" t="inlineStr">
         <is>
           <t>conf/kbse/</t>
         </is>
       </c>
-      <c r="G180" t="n">
+      <c r="G185" t="n">
         <v>2010</v>
       </c>
-      <c r="H180" t="inlineStr">
+      <c r="H185" t="inlineStr">
         <is>
           <t>conf/kbse/2010</t>
         </is>
       </c>
     </row>
-    <row r="181">
-      <c r="A181" t="inlineStr">
+    <row r="186">
+      <c r="A186" t="inlineStr">
         <is>
           <t>Yuetang Deng and Phyllis G. Frankl and Zhongqiang Chen</t>
         </is>
       </c>
-      <c r="B181" t="inlineStr">
+      <c r="B186" t="inlineStr">
         <is>
           <t>@inproceedings{deng:2003,
 booktitle = {International Conference on Automated Software Engineering(ASE)}, 
@@ -7903,42 +8128,42 @@
 }</t>
         </is>
       </c>
-      <c r="C181" t="inlineStr">
+      <c r="C186" t="inlineStr">
         <is>
           <t>conf/kbse/DengFC03</t>
         </is>
       </c>
-      <c r="D181" t="inlineStr">
+      <c r="D186" t="inlineStr">
         <is>
           <t>Testing Database Transaction Concurrency</t>
         </is>
       </c>
-      <c r="E181" t="inlineStr">
+      <c r="E186" t="inlineStr">
         <is>
           <t>db/conf/kbse/ase2003.html#DengFC03</t>
         </is>
       </c>
-      <c r="F181" t="inlineStr">
+      <c r="F186" t="inlineStr">
         <is>
           <t>conf/kbse/</t>
         </is>
       </c>
-      <c r="G181" t="n">
+      <c r="G186" t="n">
         <v>2003</v>
       </c>
-      <c r="H181" t="inlineStr">
+      <c r="H186" t="inlineStr">
         <is>
           <t>conf/kbse/2003</t>
         </is>
       </c>
     </row>
-    <row r="182">
-      <c r="A182" t="inlineStr">
+    <row r="187">
+      <c r="A187" t="inlineStr">
         <is>
           <t>Kai Pan and Xintao Wu and Tao Xie</t>
         </is>
       </c>
-      <c r="B182" t="inlineStr">
+      <c r="B187" t="inlineStr">
         <is>
           <t>@inproceedings{pan:2011,
 booktitle = {International Conference on Automated Software Engineering(ASE)}, 
@@ -7948,42 +8173,42 @@
 }</t>
         </is>
       </c>
-      <c r="C182" t="inlineStr">
+      <c r="C187" t="inlineStr">
         <is>
           <t>conf/kbse/PanWX11</t>
         </is>
       </c>
-      <c r="D182" t="inlineStr">
+      <c r="D187" t="inlineStr">
         <is>
           <t>Generating program inputs for database application testing</t>
         </is>
       </c>
-      <c r="E182" t="inlineStr">
+      <c r="E187" t="inlineStr">
         <is>
           <t>db/conf/kbse/ase2011.html#PanWX11</t>
         </is>
       </c>
-      <c r="F182" t="inlineStr">
+      <c r="F187" t="inlineStr">
         <is>
           <t>conf/kbse/</t>
         </is>
       </c>
-      <c r="G182" t="n">
+      <c r="G187" t="n">
         <v>2011</v>
       </c>
-      <c r="H182" t="inlineStr">
+      <c r="H187" t="inlineStr">
         <is>
           <t>conf/kbse/2011</t>
         </is>
       </c>
     </row>
-    <row r="183">
-      <c r="A183" t="inlineStr">
+    <row r="188">
+      <c r="A188" t="inlineStr">
         <is>
           <t>Kunal Taneja and Yi Zhang and Tao Xie 0001</t>
         </is>
       </c>
-      <c r="B183" t="inlineStr">
+      <c r="B188" t="inlineStr">
         <is>
           <t>@inproceedings{taneja:2010,
 booktitle = {International Conference on Automated Software Engineering(ASE)}, 
@@ -7993,42 +8218,42 @@
 }</t>
         </is>
       </c>
-      <c r="C183" t="inlineStr">
+      <c r="C188" t="inlineStr">
         <is>
           <t>conf/kbse/TanejaZX10</t>
         </is>
       </c>
-      <c r="D183" t="inlineStr">
+      <c r="D188" t="inlineStr">
         <is>
           <t>MODA: automated test generation for database applications via mock objects</t>
         </is>
       </c>
-      <c r="E183" t="inlineStr">
+      <c r="E188" t="inlineStr">
         <is>
           <t>db/conf/kbse/ase2010.html#TanejaZX10</t>
         </is>
       </c>
-      <c r="F183" t="inlineStr">
+      <c r="F188" t="inlineStr">
         <is>
           <t>conf/kbse/</t>
         </is>
       </c>
-      <c r="G183" t="n">
+      <c r="G188" t="n">
         <v>2010</v>
       </c>
-      <c r="H183" t="inlineStr">
+      <c r="H188" t="inlineStr">
         <is>
           <t>conf/kbse/2010</t>
         </is>
       </c>
     </row>
-    <row r="184">
-      <c r="A184" t="inlineStr">
+    <row r="189">
+      <c r="A189" t="inlineStr">
         <is>
           <t>Muhammad Suleman Mahmood and Maryam Abdul Ghafoor and Junaid Haroon Siddiqui</t>
         </is>
       </c>
-      <c r="B184" t="inlineStr">
+      <c r="B189" t="inlineStr">
         <is>
           <t>@inproceedings{suleman:2016,
 booktitle = {International Conference on Automated Software Engineering(ASE)}, 
@@ -8038,42 +8263,42 @@
 }</t>
         </is>
       </c>
-      <c r="C184" t="inlineStr">
+      <c r="C189" t="inlineStr">
         <is>
           <t>conf/kbse/MahmoodGS16</t>
         </is>
       </c>
-      <c r="D184" t="inlineStr">
+      <c r="D189" t="inlineStr">
         <is>
           <t>Symbolic execution of stored procedures in database management systems</t>
         </is>
       </c>
-      <c r="E184" t="inlineStr">
+      <c r="E189" t="inlineStr">
         <is>
           <t>db/conf/kbse/ase2016.html#MahmoodGS16</t>
         </is>
       </c>
-      <c r="F184" t="inlineStr">
+      <c r="F189" t="inlineStr">
         <is>
           <t>conf/kbse/</t>
         </is>
       </c>
-      <c r="G184" t="n">
+      <c r="G189" t="n">
         <v>2016</v>
       </c>
-      <c r="H184" t="inlineStr">
+      <c r="H189" t="inlineStr">
         <is>
           <t>conf/kbse/2016</t>
         </is>
       </c>
     </row>
-    <row r="185">
-      <c r="A185" t="inlineStr">
+    <row r="190">
+      <c r="A190" t="inlineStr">
         <is>
           <t>Hamid Ould-Brahim and Stan Matwin</t>
         </is>
       </c>
-      <c r="B185" t="inlineStr">
+      <c r="B190" t="inlineStr">
         <is>
           <t>@inproceedings{ould-brahim:1992,
 booktitle = {International Conference on Automated Software Engineering(ASE)}, 
@@ -8083,42 +8308,42 @@
 }</t>
         </is>
       </c>
-      <c r="C185" t="inlineStr">
+      <c r="C190" t="inlineStr">
         <is>
           <t>conf/kbse/Ould-BrahimM92</t>
         </is>
       </c>
-      <c r="D185" t="inlineStr">
+      <c r="D190" t="inlineStr">
         <is>
           <t>Reusing database queries in analogical domains</t>
         </is>
       </c>
-      <c r="E185" t="inlineStr">
+      <c r="E190" t="inlineStr">
         <is>
           <t>db/conf/kbse/kbse1992.html#Ould-BrahimM92</t>
         </is>
       </c>
-      <c r="F185" t="inlineStr">
+      <c r="F190" t="inlineStr">
         <is>
           <t>conf/kbse/</t>
         </is>
       </c>
-      <c r="G185" t="n">
+      <c r="G190" t="n">
         <v>1992</v>
       </c>
-      <c r="H185" t="inlineStr">
+      <c r="H190" t="inlineStr">
         <is>
           <t>conf/kbse/1992</t>
         </is>
       </c>
     </row>
-    <row r="186">
-      <c r="A186" t="inlineStr">
+    <row r="191">
+      <c r="A191" t="inlineStr">
         <is>
           <t>Mario Linares Vásquez and Boyang Li and Christopher Vendome and Denys Poshyvanyk</t>
         </is>
       </c>
-      <c r="B186" t="inlineStr">
+      <c r="B191" t="inlineStr">
         <is>
           <t>@inproceedings{linares:2015,
 booktitle = {International Conference on Automated Software Engineering(ASE)}, 
@@ -8128,42 +8353,42 @@
 }</t>
         </is>
       </c>
-      <c r="C186" t="inlineStr">
+      <c r="C191" t="inlineStr">
         <is>
           <t>conf/kbse/VasquezLVP15</t>
         </is>
       </c>
-      <c r="D186" t="inlineStr">
+      <c r="D191" t="inlineStr">
         <is>
           <t>How do Developers Document Database Usages in Source Code? (N)</t>
         </is>
       </c>
-      <c r="E186" t="inlineStr">
+      <c r="E191" t="inlineStr">
         <is>
           <t>db/conf/kbse/ase2015.html#VasquezLVP15</t>
         </is>
       </c>
-      <c r="F186" t="inlineStr">
+      <c r="F191" t="inlineStr">
         <is>
           <t>conf/kbse/</t>
         </is>
       </c>
-      <c r="G186" t="n">
+      <c r="G191" t="n">
         <v>2015</v>
       </c>
-      <c r="H186" t="inlineStr">
+      <c r="H191" t="inlineStr">
         <is>
           <t>conf/kbse/2015</t>
         </is>
       </c>
     </row>
-    <row r="187">
-      <c r="A187" t="inlineStr">
+    <row r="192">
+      <c r="A192" t="inlineStr">
         <is>
           <t>Shahrul Azman Noah and Michael D. Williams</t>
         </is>
       </c>
-      <c r="B187" t="inlineStr">
+      <c r="B192" t="inlineStr">
         <is>
           <t>@inproceedings{azman:2000,
 booktitle = {International Conference on Automated Software Engineering(ASE)}, 
@@ -8173,42 +8398,42 @@
 }</t>
         </is>
       </c>
-      <c r="C187" t="inlineStr">
+      <c r="C192" t="inlineStr">
         <is>
           <t>conf/kbse/NoahW00</t>
         </is>
       </c>
-      <c r="D187" t="inlineStr">
+      <c r="D192" t="inlineStr">
         <is>
           <t>Exploring and Validating the Contributions of Real-World Knowledge to the Diagnostic Performance of Automated Database Design Tools</t>
         </is>
       </c>
-      <c r="E187" t="inlineStr">
+      <c r="E192" t="inlineStr">
         <is>
           <t>db/conf/kbse/ase2000.html#NoahW00</t>
         </is>
       </c>
-      <c r="F187" t="inlineStr">
+      <c r="F192" t="inlineStr">
         <is>
           <t>conf/kbse/</t>
         </is>
       </c>
-      <c r="G187" t="n">
+      <c r="G192" t="n">
         <v>2000</v>
       </c>
-      <c r="H187" t="inlineStr">
+      <c r="H192" t="inlineStr">
         <is>
           <t>conf/kbse/2000</t>
         </is>
       </c>
     </row>
-    <row r="188">
-      <c r="A188" t="inlineStr">
+    <row r="193">
+      <c r="A193" t="inlineStr">
         <is>
           <t>William G. J. Halfond and Alessandro Orso</t>
         </is>
       </c>
-      <c r="B188" t="inlineStr">
+      <c r="B193" t="inlineStr">
         <is>
           <t>@inproceedings{g.:2006,
 booktitle = {International Conference on Automated Software Engineering(ASE)}, 
@@ -8218,42 +8443,42 @@
 }</t>
         </is>
       </c>
-      <c r="C188" t="inlineStr">
+      <c r="C193" t="inlineStr">
         <is>
           <t>conf/kbse/HalfondO06</t>
         </is>
       </c>
-      <c r="D188" t="inlineStr">
+      <c r="D193" t="inlineStr">
         <is>
           <t>Command-Form Coverage for Testing Database Applications</t>
         </is>
       </c>
-      <c r="E188" t="inlineStr">
+      <c r="E193" t="inlineStr">
         <is>
           <t>db/conf/kbse/ase2006.html#HalfondO06</t>
         </is>
       </c>
-      <c r="F188" t="inlineStr">
+      <c r="F193" t="inlineStr">
         <is>
           <t>conf/kbse/</t>
         </is>
       </c>
-      <c r="G188" t="n">
+      <c r="G193" t="n">
         <v>2006</v>
       </c>
-      <c r="H188" t="inlineStr">
+      <c r="H193" t="inlineStr">
         <is>
           <t>conf/kbse/2006</t>
         </is>
       </c>
     </row>
-    <row r="189">
-      <c r="A189" t="inlineStr">
+    <row r="194">
+      <c r="A194" t="inlineStr">
         <is>
           <t>Sarah R. Clark and Jake Cobb and Gregory M. Kapfhammer and James A. Jones and Mary Jean Harrold</t>
         </is>
       </c>
-      <c r="B189" t="inlineStr">
+      <c r="B194" t="inlineStr">
         <is>
           <t>@inproceedings{r.:2011,
 booktitle = {International Conference on Automated Software Engineering(ASE)}, 
@@ -8263,42 +8488,42 @@
 }</t>
         </is>
       </c>
-      <c r="C189" t="inlineStr">
+      <c r="C194" t="inlineStr">
         <is>
           <t>conf/kbse/ClarkCKJH11</t>
         </is>
       </c>
-      <c r="D189" t="inlineStr">
+      <c r="D194" t="inlineStr">
         <is>
           <t>Localizing SQL faults in database applications</t>
         </is>
       </c>
-      <c r="E189" t="inlineStr">
+      <c r="E194" t="inlineStr">
         <is>
           <t>db/conf/kbse/ase2011.html#ClarkCKJH11</t>
         </is>
       </c>
-      <c r="F189" t="inlineStr">
+      <c r="F194" t="inlineStr">
         <is>
           <t>conf/kbse/</t>
         </is>
       </c>
-      <c r="G189" t="n">
+      <c r="G194" t="n">
         <v>2011</v>
       </c>
-      <c r="H189" t="inlineStr">
+      <c r="H194" t="inlineStr">
         <is>
           <t>conf/kbse/2011</t>
         </is>
       </c>
     </row>
-    <row r="190">
-      <c r="A190" t="inlineStr">
+    <row r="195">
+      <c r="A195" t="inlineStr">
         <is>
           <t>Yuetang Deng and Phyllis G. Frankl and David Chays</t>
         </is>
       </c>
-      <c r="B190" t="inlineStr">
+      <c r="B195" t="inlineStr">
         <is>
           <t>@inproceedings{deng:2005,
 booktitle = {International Conference on Software Engineering (ICSE)}, 
@@ -8308,42 +8533,42 @@
 }</t>
         </is>
       </c>
-      <c r="C190" t="inlineStr">
+      <c r="C195" t="inlineStr">
         <is>
           <t>conf/icse/DengFC05</t>
         </is>
       </c>
-      <c r="D190" t="inlineStr">
+      <c r="D195" t="inlineStr">
         <is>
           <t>Testing database transactions with AGENDA</t>
         </is>
       </c>
-      <c r="E190" t="inlineStr">
+      <c r="E195" t="inlineStr">
         <is>
           <t>db/conf/icse/icse2005.html#DengFC05</t>
         </is>
       </c>
-      <c r="F190" t="inlineStr">
+      <c r="F195" t="inlineStr">
         <is>
           <t>conf/icse/</t>
         </is>
       </c>
-      <c r="G190" t="n">
+      <c r="G195" t="n">
         <v>2005</v>
       </c>
-      <c r="H190" t="inlineStr">
+      <c r="H195" t="inlineStr">
         <is>
           <t>conf/icse/2005</t>
         </is>
       </c>
     </row>
-    <row r="191">
-      <c r="A191" t="inlineStr">
+    <row r="196">
+      <c r="A196" t="inlineStr">
         <is>
           <t>Mathieu Humblet and Dang Vinh Tran and Jens H. Weber and Anthony Cleve</t>
         </is>
       </c>
-      <c r="B191" t="inlineStr">
+      <c r="B196" t="inlineStr">
         <is>
           <t>@inproceedings{humblet:2016,
 booktitle = {International Conference on Software Engineering (ICSE)}, 
@@ -8353,42 +8578,42 @@
 }</t>
         </is>
       </c>
-      <c r="C191" t="inlineStr">
+      <c r="C196" t="inlineStr">
         <is>
           <t>conf/icse/HumbletTWC16</t>
         </is>
       </c>
-      <c r="D191" t="inlineStr">
+      <c r="D196" t="inlineStr">
         <is>
           <t>Variability management in database applications</t>
         </is>
       </c>
-      <c r="E191" t="inlineStr">
+      <c r="E196" t="inlineStr">
         <is>
           <t>db/conf/icse/vace2016.html#HumbletTWC16</t>
         </is>
       </c>
-      <c r="F191" t="inlineStr">
+      <c r="F196" t="inlineStr">
         <is>
           <t>conf/icse/</t>
         </is>
       </c>
-      <c r="G191" t="n">
+      <c r="G196" t="n">
         <v>2016</v>
       </c>
-      <c r="H191" t="inlineStr">
+      <c r="H196" t="inlineStr">
         <is>
           <t>conf/icse/2016vace</t>
         </is>
       </c>
     </row>
-    <row r="192">
-      <c r="A192" t="inlineStr">
+    <row r="197">
+      <c r="A197" t="inlineStr">
         <is>
           <t>Klaus R. Dittrich and Dimitris Tombros and Andreas Geppert</t>
         </is>
       </c>
-      <c r="B192" t="inlineStr">
+      <c r="B197" t="inlineStr">
         <is>
           <t>@inproceedings{r.:2000,
 booktitle = {International Conference on Software Engineering (ICSE)}, 
@@ -8398,42 +8623,42 @@
 }</t>
         </is>
       </c>
-      <c r="C192" t="inlineStr">
+      <c r="C197" t="inlineStr">
         <is>
           <t>conf/icse/DittrichTG00</t>
         </is>
       </c>
-      <c r="D192" t="inlineStr">
+      <c r="D197" t="inlineStr">
         <is>
           <t>Databases in software engineering: a roadmap</t>
         </is>
       </c>
-      <c r="E192" t="inlineStr">
+      <c r="E197" t="inlineStr">
         <is>
           <t>db/conf/icse/future2000.html#DittrichTG00</t>
         </is>
       </c>
-      <c r="F192" t="inlineStr">
+      <c r="F197" t="inlineStr">
         <is>
           <t>conf/icse/</t>
         </is>
       </c>
-      <c r="G192" t="n">
+      <c r="G197" t="n">
         <v>2000</v>
       </c>
-      <c r="H192" t="inlineStr">
+      <c r="H197" t="inlineStr">
         <is>
           <t>conf/icse/2000future</t>
         </is>
       </c>
     </row>
-    <row r="193">
-      <c r="A193" t="inlineStr">
+    <row r="198">
+      <c r="A198" t="inlineStr">
         <is>
           <t>Andy Maule and Wolfgang Emmerich and David S. Rosenblum</t>
         </is>
       </c>
-      <c r="B193" t="inlineStr">
+      <c r="B198" t="inlineStr">
         <is>
           <t>@inproceedings{maule:2008,
 booktitle = {International Conference on Software Engineering (ICSE)}, 
@@ -8443,42 +8668,42 @@
 }</t>
         </is>
       </c>
-      <c r="C193" t="inlineStr">
+      <c r="C198" t="inlineStr">
         <is>
           <t>conf/icse/MauleER08</t>
         </is>
       </c>
-      <c r="D193" t="inlineStr">
+      <c r="D198" t="inlineStr">
         <is>
           <t>Impact analysis of database schema changes</t>
         </is>
       </c>
-      <c r="E193" t="inlineStr">
+      <c r="E198" t="inlineStr">
         <is>
           <t>db/conf/icse/icse2008.html#MauleER08</t>
         </is>
       </c>
-      <c r="F193" t="inlineStr">
+      <c r="F198" t="inlineStr">
         <is>
           <t>conf/icse/</t>
         </is>
       </c>
-      <c r="G193" t="n">
+      <c r="G198" t="n">
         <v>2008</v>
       </c>
-      <c r="H193" t="inlineStr">
+      <c r="H198" t="inlineStr">
         <is>
           <t>conf/icse/2008</t>
         </is>
       </c>
     </row>
-    <row r="194">
-      <c r="A194" t="inlineStr">
+    <row r="199">
+      <c r="A199" t="inlineStr">
         <is>
           <t>Roger King</t>
         </is>
       </c>
-      <c r="B194" t="inlineStr">
+      <c r="B199" t="inlineStr">
         <is>
           <t>@inproceedings{king:1994,
 booktitle = {International Conference on Software Engineering (ICSE)}, 
@@ -8488,42 +8713,42 @@
 }</t>
         </is>
       </c>
-      <c r="C194" t="inlineStr">
+      <c r="C199" t="inlineStr">
         <is>
           <t>conf/icse/King94</t>
         </is>
       </c>
-      <c r="D194" t="inlineStr">
+      <c r="D199" t="inlineStr">
         <is>
           <t>Workshop on the Intersection Between Databases and Software Engineering</t>
         </is>
       </c>
-      <c r="E194" t="inlineStr">
+      <c r="E199" t="inlineStr">
         <is>
           <t>db/conf/icse/icse94.html#King94</t>
         </is>
       </c>
-      <c r="F194" t="inlineStr">
+      <c r="F199" t="inlineStr">
         <is>
           <t>conf/icse/</t>
         </is>
       </c>
-      <c r="G194" t="n">
+      <c r="G199" t="n">
         <v>1994</v>
       </c>
-      <c r="H194" t="inlineStr">
+      <c r="H199" t="inlineStr">
         <is>
           <t>conf/icse/1994</t>
         </is>
       </c>
     </row>
-    <row r="195">
-      <c r="A195" t="inlineStr">
+    <row r="200">
+      <c r="A200" t="inlineStr">
         <is>
           <t>John Slankas</t>
         </is>
       </c>
-      <c r="B195" t="inlineStr">
+      <c r="B200" t="inlineStr">
         <is>
           <t>@inproceedings{slankas:2013,
 booktitle = {International Conference on Software Engineering (ICSE)}, 
@@ -8533,42 +8758,42 @@
 }</t>
         </is>
       </c>
-      <c r="C195" t="inlineStr">
+      <c r="C200" t="inlineStr">
         <is>
           <t>conf/icse/Slankas04</t>
         </is>
       </c>
-      <c r="D195" t="inlineStr">
+      <c r="D200" t="inlineStr">
         <is>
           <t>Implementing database access control policy from unconstrained natural language text</t>
         </is>
       </c>
-      <c r="E195" t="inlineStr">
+      <c r="E200" t="inlineStr">
         <is>
           <t>db/conf/icse/icse2013.html#Slankas04</t>
         </is>
       </c>
-      <c r="F195" t="inlineStr">
+      <c r="F200" t="inlineStr">
         <is>
           <t>conf/icse/</t>
         </is>
       </c>
-      <c r="G195" t="n">
+      <c r="G200" t="n">
         <v>2013</v>
       </c>
-      <c r="H195" t="inlineStr">
+      <c r="H200" t="inlineStr">
         <is>
           <t>conf/icse/2013</t>
         </is>
       </c>
     </row>
-    <row r="196">
-      <c r="A196" t="inlineStr">
+    <row r="201">
+      <c r="A201" t="inlineStr">
         <is>
           <t>Wito Delnat and Eddy Truyen and Ansar Rafique and Dimitri Van Landuyt and Wouter Joosen</t>
         </is>
       </c>
-      <c r="B196" t="inlineStr">
+      <c r="B201" t="inlineStr">
         <is>
           <t>@inproceedings{delnat:2018,
 booktitle = {International Conference on Software Engineering (ICSE)}, 
@@ -8578,42 +8803,42 @@
 }</t>
         </is>
       </c>
-      <c r="C196" t="inlineStr">
+      <c r="C201" t="inlineStr">
         <is>
           <t>conf/icse/DelnatTRLJ18</t>
         </is>
       </c>
-      <c r="D196" t="inlineStr">
+      <c r="D201" t="inlineStr">
         <is>
           <t>K8-scalar: a workbench to compare autoscalers for container-orchestrated database clusters</t>
         </is>
       </c>
-      <c r="E196" t="inlineStr">
+      <c r="E201" t="inlineStr">
         <is>
           <t>db/conf/icse/seams2018.html#DelnatTRLJ18</t>
         </is>
       </c>
-      <c r="F196" t="inlineStr">
+      <c r="F201" t="inlineStr">
         <is>
           <t>conf/icse/</t>
         </is>
       </c>
-      <c r="G196" t="n">
+      <c r="G201" t="n">
         <v>2018</v>
       </c>
-      <c r="H196" t="inlineStr">
+      <c r="H201" t="inlineStr">
         <is>
           <t>conf/icse/2018seams</t>
         </is>
       </c>
     </row>
-    <row r="197">
-      <c r="A197" t="inlineStr">
+    <row r="202">
+      <c r="A202" t="inlineStr">
         <is>
           <t>Philip A. Bernstein</t>
         </is>
       </c>
-      <c r="B197" t="inlineStr">
+      <c r="B202" t="inlineStr">
         <is>
           <t>@inproceedings{a.:1987,
 booktitle = {International Conference on Software Engineering (ICSE)}, 
@@ -8623,42 +8848,42 @@
 }</t>
         </is>
       </c>
-      <c r="C197" t="inlineStr">
+      <c r="C202" t="inlineStr">
         <is>
           <t>conf/icse/Bernstein87</t>
         </is>
       </c>
-      <c r="D197" t="inlineStr">
+      <c r="D202" t="inlineStr">
         <is>
           <t>Database System Support for Software Engineering</t>
         </is>
       </c>
-      <c r="E197" t="inlineStr">
+      <c r="E202" t="inlineStr">
         <is>
           <t>db/conf/icse/icse87.html#Bernstein87</t>
         </is>
       </c>
-      <c r="F197" t="inlineStr">
+      <c r="F202" t="inlineStr">
         <is>
           <t>conf/icse/</t>
         </is>
       </c>
-      <c r="G197" t="n">
+      <c r="G202" t="n">
         <v>1987</v>
       </c>
-      <c r="H197" t="inlineStr">
+      <c r="H202" t="inlineStr">
         <is>
           <t>conf/icse/1987</t>
         </is>
       </c>
     </row>
-    <row r="198">
-      <c r="A198" t="inlineStr">
+    <row r="203">
+      <c r="A203" t="inlineStr">
         <is>
           <t>Tse-Hsun Chen and Weiyi Shang and Ahmed E. Hassan and Mohamed N. Nasser and Parminder Flora</t>
         </is>
       </c>
-      <c r="B198" t="inlineStr">
+      <c r="B203" t="inlineStr">
         <is>
           <t>@inproceedings{chen:2016,
 booktitle = {International Conference on Software Engineering (ICSE)}, 
@@ -8668,42 +8893,42 @@
 }</t>
         </is>
       </c>
-      <c r="C198" t="inlineStr">
+      <c r="C203" t="inlineStr">
         <is>
           <t>conf/icse/ChenSHNF16</t>
         </is>
       </c>
-      <c r="D198" t="inlineStr">
+      <c r="D203" t="inlineStr">
         <is>
           <t>Detecting problems in the database access code of large scale systems: an industrial experience report</t>
         </is>
       </c>
-      <c r="E198" t="inlineStr">
+      <c r="E203" t="inlineStr">
         <is>
           <t>db/conf/icse/icse2016c.html#ChenSHNF16</t>
         </is>
       </c>
-      <c r="F198" t="inlineStr">
+      <c r="F203" t="inlineStr">
         <is>
           <t>conf/icse/</t>
         </is>
       </c>
-      <c r="G198" t="n">
+      <c r="G203" t="n">
         <v>2016</v>
       </c>
-      <c r="H198" t="inlineStr">
+      <c r="H203" t="inlineStr">
         <is>
           <t>conf/icse/2016c</t>
         </is>
       </c>
     </row>
-    <row r="199">
-      <c r="A199" t="inlineStr">
+    <row r="204">
+      <c r="A204" t="inlineStr">
         <is>
           <t>Rudolf Bayer</t>
         </is>
       </c>
-      <c r="B199" t="inlineStr">
+      <c r="B204" t="inlineStr">
         <is>
           <t>@inproceedings{bayer:1979,
 booktitle = {International Conference on Software Engineering (ICSE)}, 
@@ -8713,42 +8938,42 @@
 }</t>
         </is>
       </c>
-      <c r="C199" t="inlineStr">
+      <c r="C204" t="inlineStr">
         <is>
           <t>conf/icse/Bayer79</t>
         </is>
       </c>
-      <c r="D199" t="inlineStr">
+      <c r="D204" t="inlineStr">
         <is>
           <t>On Synchronization and Recovery in Database Systems</t>
         </is>
       </c>
-      <c r="E199" t="inlineStr">
+      <c r="E204" t="inlineStr">
         <is>
           <t>db/conf/icse/icse79.html#Bayer79</t>
         </is>
       </c>
-      <c r="F199" t="inlineStr">
+      <c r="F204" t="inlineStr">
         <is>
           <t>conf/icse/</t>
         </is>
       </c>
-      <c r="G199" t="n">
+      <c r="G204" t="n">
         <v>1979</v>
       </c>
-      <c r="H199" t="inlineStr">
+      <c r="H204" t="inlineStr">
         <is>
           <t>conf/icse/1979</t>
         </is>
       </c>
     </row>
-    <row r="200">
-      <c r="A200" t="inlineStr">
+    <row r="205">
+      <c r="A205" t="inlineStr">
         <is>
           <t>David Willmor and Suzanne M. Embury</t>
         </is>
       </c>
-      <c r="B200" t="inlineStr">
+      <c r="B205" t="inlineStr">
         <is>
           <t>@inproceedings{willmor:2006,
 booktitle = {International Conference on Software Engineering (ICSE)}, 
@@ -8758,42 +8983,42 @@
 }</t>
         </is>
       </c>
-      <c r="C200" t="inlineStr">
+      <c r="C205" t="inlineStr">
         <is>
           <t>conf/icse/WillmorE06</t>
         </is>
       </c>
-      <c r="D200" t="inlineStr">
+      <c r="D205" t="inlineStr">
         <is>
           <t>An intensional approach to the specification of test cases for database applications</t>
         </is>
       </c>
-      <c r="E200" t="inlineStr">
+      <c r="E205" t="inlineStr">
         <is>
           <t>db/conf/icse/icse2006.html#WillmorE06</t>
         </is>
       </c>
-      <c r="F200" t="inlineStr">
+      <c r="F205" t="inlineStr">
         <is>
           <t>conf/icse/</t>
         </is>
       </c>
-      <c r="G200" t="n">
+      <c r="G205" t="n">
         <v>2006</v>
       </c>
-      <c r="H200" t="inlineStr">
+      <c r="H205" t="inlineStr">
         <is>
           <t>conf/icse/2006</t>
         </is>
       </c>
     </row>
-    <row r="201">
-      <c r="A201" t="inlineStr">
+    <row r="206">
+      <c r="A206" t="inlineStr">
         <is>
           <t>Karen E. Huff</t>
         </is>
       </c>
-      <c r="B201" t="inlineStr">
+      <c r="B206" t="inlineStr">
         <is>
           <t>@inproceedings{e.:1981,
 booktitle = {International Conference on Software Engineering (ICSE)}, 
@@ -8803,42 +9028,42 @@
 }</t>
         </is>
       </c>
-      <c r="C201" t="inlineStr">
+      <c r="C206" t="inlineStr">
         <is>
           <t>conf/icse/Huff81</t>
         </is>
       </c>
-      <c r="D201" t="inlineStr">
+      <c r="D206" t="inlineStr">
         <is>
           <t>A Database Model for Effective Configuration Management in the Programming Environment</t>
         </is>
       </c>
-      <c r="E201" t="inlineStr">
+      <c r="E206" t="inlineStr">
         <is>
           <t>db/conf/icse/icse81.html#Huff81</t>
         </is>
       </c>
-      <c r="F201" t="inlineStr">
+      <c r="F206" t="inlineStr">
         <is>
           <t>conf/icse/</t>
         </is>
       </c>
-      <c r="G201" t="n">
+      <c r="G206" t="n">
         <v>1981</v>
       </c>
-      <c r="H201" t="inlineStr">
+      <c r="H206" t="inlineStr">
         <is>
           <t>conf/icse/1981</t>
         </is>
       </c>
     </row>
-    <row r="202">
-      <c r="A202" t="inlineStr">
+    <row r="207">
+      <c r="A207" t="inlineStr">
         <is>
           <t>Kai Pan and Xintao Wu and Tao Xie</t>
         </is>
       </c>
-      <c r="B202" t="inlineStr">
+      <c r="B207" t="inlineStr">
         <is>
           <t>@inproceedings{pan:2013,
 booktitle = {International Conference on Software Engineering (ICSE)}, 
@@ -8848,42 +9073,42 @@
 }</t>
         </is>
       </c>
-      <c r="C202" t="inlineStr">
+      <c r="C207" t="inlineStr">
         <is>
           <t>conf/icse/PanWX13</t>
         </is>
       </c>
-      <c r="D202" t="inlineStr">
+      <c r="D207" t="inlineStr">
         <is>
           <t>Automatic test generation for mutation testing on database applications</t>
         </is>
       </c>
-      <c r="E202" t="inlineStr">
+      <c r="E207" t="inlineStr">
         <is>
           <t>db/conf/icse/ast2013.html#PanWX13</t>
         </is>
       </c>
-      <c r="F202" t="inlineStr">
+      <c r="F207" t="inlineStr">
         <is>
           <t>conf/icse/</t>
         </is>
       </c>
-      <c r="G202" t="n">
+      <c r="G207" t="n">
         <v>2013</v>
       </c>
-      <c r="H202" t="inlineStr">
+      <c r="H207" t="inlineStr">
         <is>
           <t>conf/icse/2013ast</t>
         </is>
       </c>
     </row>
-    <row r="203">
-      <c r="A203" t="inlineStr">
+    <row r="208">
+      <c r="A208" t="inlineStr">
         <is>
           <t>Mashel Al-Barak and Rami Bahsoon</t>
         </is>
       </c>
-      <c r="B203" t="inlineStr">
+      <c r="B208" t="inlineStr">
         <is>
           <t>@inproceedings{al-barak:2018,
 booktitle = {International Conference on Software Engineering (ICSE)}, 
@@ -8893,42 +9118,42 @@
 }</t>
         </is>
       </c>
-      <c r="C203" t="inlineStr">
+      <c r="C208" t="inlineStr">
         <is>
           <t>conf/icse/Al-BarakB18</t>
         </is>
       </c>
-      <c r="D203" t="inlineStr">
+      <c r="D208" t="inlineStr">
         <is>
           <t>Prioritizing technical debt in database normalization using portfolio theory and data quality metrics</t>
         </is>
       </c>
-      <c r="E203" t="inlineStr">
+      <c r="E208" t="inlineStr">
         <is>
           <t>db/conf/icse/techdebt2018.html#Al-BarakB18</t>
         </is>
       </c>
-      <c r="F203" t="inlineStr">
+      <c r="F208" t="inlineStr">
         <is>
           <t>conf/icse/</t>
         </is>
       </c>
-      <c r="G203" t="n">
+      <c r="G208" t="n">
         <v>2018</v>
       </c>
-      <c r="H203" t="inlineStr">
+      <c r="H208" t="inlineStr">
         <is>
           <t>conf/icse/2018techdebt</t>
         </is>
       </c>
     </row>
-    <row r="204">
-      <c r="A204" t="inlineStr">
+    <row r="209">
+      <c r="A209" t="inlineStr">
         <is>
           <t>David Chays and Yuetang Deng</t>
         </is>
       </c>
-      <c r="B204" t="inlineStr">
+      <c r="B209" t="inlineStr">
         <is>
           <t>@inproceedings{chays:2003,
 booktitle = {International Conference on Software Engineering (ICSE)}, 
@@ -8938,42 +9163,42 @@
 }</t>
         </is>
       </c>
-      <c r="C204" t="inlineStr">
+      <c r="C209" t="inlineStr">
         <is>
           <t>conf/icse/ChaysD03</t>
         </is>
       </c>
-      <c r="D204" t="inlineStr">
+      <c r="D209" t="inlineStr">
         <is>
           <t>Demonstration of AGENDA Tool Set for Testing Relational Database Applications</t>
         </is>
       </c>
-      <c r="E204" t="inlineStr">
+      <c r="E209" t="inlineStr">
         <is>
           <t>db/conf/icse/icse2003.html#ChaysD03</t>
         </is>
       </c>
-      <c r="F204" t="inlineStr">
+      <c r="F209" t="inlineStr">
         <is>
           <t>conf/icse/</t>
         </is>
       </c>
-      <c r="G204" t="n">
+      <c r="G209" t="n">
         <v>2003</v>
       </c>
-      <c r="H204" t="inlineStr">
+      <c r="H209" t="inlineStr">
         <is>
           <t>conf/icse/2003</t>
         </is>
       </c>
     </row>
-    <row r="205">
-      <c r="A205" t="inlineStr">
+    <row r="210">
+      <c r="A210" t="inlineStr">
         <is>
           <t>Richard W. Selby</t>
         </is>
       </c>
-      <c r="B205" t="inlineStr">
+      <c r="B210" t="inlineStr">
         <is>
           <t>@inproceedings{w.:1997,
 booktitle = {International Conference on Software Engineering (ICSE)}, 
@@ -8983,42 +9208,42 @@
 }</t>
         </is>
       </c>
-      <c r="C205" t="inlineStr">
+      <c r="C210" t="inlineStr">
         <is>
           <t>conf/icse/Selby97</t>
         </is>
       </c>
-      <c r="D205" t="inlineStr">
+      <c r="D210" t="inlineStr">
         <is>
           <t>Platforms for Software Execution: Databases vs. Operating Systems vs. Browsers (Panel)</t>
         </is>
       </c>
-      <c r="E205" t="inlineStr">
+      <c r="E210" t="inlineStr">
         <is>
           <t>db/conf/icse/icse97.html#Selby97</t>
         </is>
       </c>
-      <c r="F205" t="inlineStr">
+      <c r="F210" t="inlineStr">
         <is>
           <t>conf/icse/</t>
         </is>
       </c>
-      <c r="G205" t="n">
+      <c r="G210" t="n">
         <v>1997</v>
       </c>
-      <c r="H205" t="inlineStr">
+      <c r="H210" t="inlineStr">
         <is>
           <t>conf/icse/1997</t>
         </is>
       </c>
     </row>
-    <row r="206">
-      <c r="A206" t="inlineStr">
+    <row r="211">
+      <c r="A211" t="inlineStr">
         <is>
           <t>Isao Miyamoto</t>
         </is>
       </c>
-      <c r="B206" t="inlineStr">
+      <c r="B211" t="inlineStr">
         <is>
           <t>@inproceedings{miyamoto:1976,
 booktitle = {International Conference on Software Engineering (ICSE)}, 
@@ -9028,42 +9253,42 @@
 }</t>
         </is>
       </c>
-      <c r="C206" t="inlineStr">
+      <c r="C211" t="inlineStr">
         <is>
           <t>conf/icse/Miyamoto76</t>
         </is>
       </c>
-      <c r="D206" t="inlineStr">
+      <c r="D211" t="inlineStr">
         <is>
           <t>Some Considerations in Database Application Programming</t>
         </is>
       </c>
-      <c r="E206" t="inlineStr">
+      <c r="E211" t="inlineStr">
         <is>
           <t>db/conf/icse/icse76.html#Miyamoto76</t>
         </is>
       </c>
-      <c r="F206" t="inlineStr">
+      <c r="F211" t="inlineStr">
         <is>
           <t>conf/icse/</t>
         </is>
       </c>
-      <c r="G206" t="n">
+      <c r="G211" t="n">
         <v>1976</v>
       </c>
-      <c r="H206" t="inlineStr">
+      <c r="H211" t="inlineStr">
         <is>
           <t>conf/icse/1976</t>
         </is>
       </c>
     </row>
-    <row r="207">
-      <c r="A207" t="inlineStr">
+    <row r="212">
+      <c r="A212" t="inlineStr">
         <is>
           <t>Andreza M. F. V. de Castro and Gisele Macedo and Eliane Collins and Arilo Claudio Dias-Neto</t>
         </is>
       </c>
-      <c r="B207" t="inlineStr">
+      <c r="B212" t="inlineStr">
         <is>
           <t>@inproceedings{m.:2013,
 booktitle = {International Conference on Software Engineering (ICSE)}, 
@@ -9073,42 +9298,42 @@
 }</t>
         </is>
       </c>
-      <c r="C207" t="inlineStr">
+      <c r="C212" t="inlineStr">
         <is>
           <t>conf/icse/CastroMCD13</t>
         </is>
       </c>
-      <c r="D207" t="inlineStr">
+      <c r="D212" t="inlineStr">
         <is>
           <t>Extension of Selenium RC tool to perform automated testing with databases in web applications</t>
         </is>
       </c>
-      <c r="E207" t="inlineStr">
+      <c r="E212" t="inlineStr">
         <is>
           <t>db/conf/icse/ast2013.html#CastroMCD13</t>
         </is>
       </c>
-      <c r="F207" t="inlineStr">
+      <c r="F212" t="inlineStr">
         <is>
           <t>conf/icse/</t>
         </is>
       </c>
-      <c r="G207" t="n">
+      <c r="G212" t="n">
         <v>2013</v>
       </c>
-      <c r="H207" t="inlineStr">
+      <c r="H212" t="inlineStr">
         <is>
           <t>conf/icse/2013ast</t>
         </is>
       </c>
     </row>
-    <row r="208">
-      <c r="A208" t="inlineStr">
+    <row r="213">
+      <c r="A213" t="inlineStr">
         <is>
           <t>Cathrin Weiss and Cindy Rubio-González and Ben Liblit</t>
         </is>
       </c>
-      <c r="B208" t="inlineStr">
+      <c r="B213" t="inlineStr">
         <is>
           <t>@inproceedings{weiss:2015,
 booktitle = {International Conference on Software Engineering (ICSE)}, 
@@ -9118,42 +9343,42 @@
 }</t>
         </is>
       </c>
-      <c r="C208" t="inlineStr">
+      <c r="C213" t="inlineStr">
         <is>
           <t>conf/icse/WeissRL15</t>
         </is>
       </c>
-      <c r="D208" t="inlineStr">
+      <c r="D213" t="inlineStr">
         <is>
           <t>Database-Backed Program Analysis for Scalable Error Propagation</t>
         </is>
       </c>
-      <c r="E208" t="inlineStr">
+      <c r="E213" t="inlineStr">
         <is>
           <t>db/conf/icse/icse2015-1.html#WeissRL15</t>
         </is>
       </c>
-      <c r="F208" t="inlineStr">
+      <c r="F213" t="inlineStr">
         <is>
           <t>conf/icse/</t>
         </is>
       </c>
-      <c r="G208" t="n">
+      <c r="G213" t="n">
         <v>2015</v>
       </c>
-      <c r="H208" t="inlineStr">
+      <c r="H213" t="inlineStr">
         <is>
           <t>conf/icse/2015-1</t>
         </is>
       </c>
     </row>
-    <row r="209">
-      <c r="A209" t="inlineStr">
+    <row r="214">
+      <c r="A214" t="inlineStr">
         <is>
           <t>Dimitrios S. Kolovos and Fady Medhat and Richard F. Paige and Davide Di Ruscio and Tijs van der Storm and Sebastian Scholze and Athanasios Zolotas</t>
         </is>
       </c>
-      <c r="B209" t="inlineStr">
+      <c r="B214" t="inlineStr">
         <is>
           <t>@inproceedings{s.:2019,
 booktitle = {International Conference on Software Engineering (ICSE)}, 
@@ -9163,42 +9388,42 @@
 }</t>
         </is>
       </c>
-      <c r="C209" t="inlineStr">
+      <c r="C214" t="inlineStr">
         <is>
           <t>conf/icse/KolovosMPRSSZ19</t>
         </is>
       </c>
-      <c r="D209" t="inlineStr">
+      <c r="D214" t="inlineStr">
         <is>
           <t>Domain-specific languages for the design, deployment and manipulation of heterogeneous databases</t>
         </is>
       </c>
-      <c r="E209" t="inlineStr">
+      <c r="E214" t="inlineStr">
         <is>
           <t>db/conf/icse/mise2019.html#KolovosMPRSSZ19</t>
         </is>
       </c>
-      <c r="F209" t="inlineStr">
+      <c r="F214" t="inlineStr">
         <is>
           <t>conf/icse/</t>
         </is>
       </c>
-      <c r="G209" t="n">
+      <c r="G214" t="n">
         <v>2019</v>
       </c>
-      <c r="H209" t="inlineStr">
+      <c r="H214" t="inlineStr">
         <is>
           <t>conf/icse/2019mise</t>
         </is>
       </c>
     </row>
-    <row r="210">
-      <c r="A210" t="inlineStr">
+    <row r="215">
+      <c r="A215" t="inlineStr">
         <is>
           <t>Maria Heloisa (Lolo) Penedo and E. Don Stuckle</t>
         </is>
       </c>
-      <c r="B210" t="inlineStr">
+      <c r="B215" t="inlineStr">
         <is>
           <t>@inproceedings{heloisa:1985,
 booktitle = {International Conference on Software Engineering (ICSE)}, 
@@ -9208,42 +9433,42 @@
 }</t>
         </is>
       </c>
-      <c r="C210" t="inlineStr">
+      <c r="C215" t="inlineStr">
         <is>
           <t>conf/icse/PenedoS85</t>
         </is>
       </c>
-      <c r="D210" t="inlineStr">
+      <c r="D215" t="inlineStr">
         <is>
           <t>PMDB - A Project Master Database for Software Engineering Environments</t>
         </is>
       </c>
-      <c r="E210" t="inlineStr">
+      <c r="E215" t="inlineStr">
         <is>
           <t>db/conf/icse/icse85.html#PenedoS85</t>
         </is>
       </c>
-      <c r="F210" t="inlineStr">
+      <c r="F215" t="inlineStr">
         <is>
           <t>conf/icse/</t>
         </is>
       </c>
-      <c r="G210" t="n">
+      <c r="G215" t="n">
         <v>1985</v>
       </c>
-      <c r="H210" t="inlineStr">
+      <c r="H215" t="inlineStr">
         <is>
           <t>conf/icse/1985</t>
         </is>
       </c>
     </row>
-    <row r="211">
-      <c r="A211" t="inlineStr">
+    <row r="216">
+      <c r="A216" t="inlineStr">
         <is>
           <t>K. Chong and P. Hsia</t>
         </is>
       </c>
-      <c r="B211" t="inlineStr">
+      <c r="B216" t="inlineStr">
         <is>
           <t>@inproceedings{chong:1984,
 booktitle = {International Conference on Software Engineering (ICSE)}, 
@@ -9253,42 +9478,42 @@
 }</t>
         </is>
       </c>
-      <c r="C211" t="inlineStr">
+      <c r="C216" t="inlineStr">
         <is>
           <t>conf/icse/ChongH84</t>
         </is>
       </c>
-      <c r="D211" t="inlineStr">
+      <c r="D216" t="inlineStr">
         <is>
           <t>Diagnostic System for Distributed Software: A Relational Database Approach</t>
         </is>
       </c>
-      <c r="E211" t="inlineStr">
+      <c r="E216" t="inlineStr">
         <is>
           <t>db/conf/icse/icse84.html#ChongH84</t>
         </is>
       </c>
-      <c r="F211" t="inlineStr">
+      <c r="F216" t="inlineStr">
         <is>
           <t>conf/icse/</t>
         </is>
       </c>
-      <c r="G211" t="n">
+      <c r="G216" t="n">
         <v>1984</v>
       </c>
-      <c r="H211" t="inlineStr">
+      <c r="H216" t="inlineStr">
         <is>
           <t>conf/icse/1984</t>
         </is>
       </c>
     </row>
-    <row r="212">
-      <c r="A212" t="inlineStr">
+    <row r="217">
+      <c r="A217" t="inlineStr">
         <is>
           <t>David W. Stemple and Tim Sheard</t>
         </is>
       </c>
-      <c r="B212" t="inlineStr">
+      <c r="B217" t="inlineStr">
         <is>
           <t>@inproceedings{w.:1985,
 booktitle = {International Conference on Software Engineering (ICSE)}, 
@@ -9298,42 +9523,42 @@
 }</t>
         </is>
       </c>
-      <c r="C212" t="inlineStr">
+      <c r="C217" t="inlineStr">
         <is>
           <t>conf/icse/StempleS85</t>
         </is>
       </c>
-      <c r="D212" t="inlineStr">
+      <c r="D217" t="inlineStr">
         <is>
           <t>Database Theory for Supporting Specification-Based Database Systems Development</t>
         </is>
       </c>
-      <c r="E212" t="inlineStr">
+      <c r="E217" t="inlineStr">
         <is>
           <t>db/conf/icse/icse85.html#StempleS85</t>
         </is>
       </c>
-      <c r="F212" t="inlineStr">
+      <c r="F217" t="inlineStr">
         <is>
           <t>conf/icse/</t>
         </is>
       </c>
-      <c r="G212" t="n">
+      <c r="G217" t="n">
         <v>1985</v>
       </c>
-      <c r="H212" t="inlineStr">
+      <c r="H217" t="inlineStr">
         <is>
           <t>conf/icse/1985</t>
         </is>
       </c>
     </row>
-    <row r="213">
-      <c r="A213" t="inlineStr">
+    <row r="218">
+      <c r="A218" t="inlineStr">
         <is>
           <t>Marco Scavuzzo and Damian Andrew Tamburri and Elisabetta Di Nitto</t>
         </is>
       </c>
-      <c r="B213" t="inlineStr">
+      <c r="B218" t="inlineStr">
         <is>
           <t>@inproceedings{scavuzzo:2016,
 booktitle = {International Conference on Software Engineering (ICSE)}, 
@@ -9343,42 +9568,42 @@
 }</t>
         </is>
       </c>
-      <c r="C213" t="inlineStr">
+      <c r="C218" t="inlineStr">
         <is>
           <t>conf/icse/ScavuzzoTN16</t>
         </is>
       </c>
-      <c r="D213" t="inlineStr">
+      <c r="D218" t="inlineStr">
         <is>
           <t>Providing big data applications with fault-tolerant data migration across heterogeneous NoSQL databases</t>
         </is>
       </c>
-      <c r="E213" t="inlineStr">
+      <c r="E218" t="inlineStr">
         <is>
           <t>db/conf/icse/bigdse2016.html#ScavuzzoTN16</t>
         </is>
       </c>
-      <c r="F213" t="inlineStr">
+      <c r="F218" t="inlineStr">
         <is>
           <t>conf/icse/</t>
         </is>
       </c>
-      <c r="G213" t="n">
+      <c r="G218" t="n">
         <v>2016</v>
       </c>
-      <c r="H213" t="inlineStr">
+      <c r="H218" t="inlineStr">
         <is>
           <t>conf/icse/2016bigdse</t>
         </is>
       </c>
     </row>
-    <row r="214">
-      <c r="A214" t="inlineStr">
+    <row r="219">
+      <c r="A219" t="inlineStr">
         <is>
           <t>Jaumir V. da Silveira Jr. and Karin Koogan Breitman</t>
         </is>
       </c>
-      <c r="B214" t="inlineStr">
+      <c r="B219" t="inlineStr">
         <is>
           <t>@inproceedings{v.:2011,
 booktitle = {International Conference on Software Engineering (ICSE)}, 
@@ -9388,42 +9613,42 @@
 }</t>
         </is>
       </c>
-      <c r="C214" t="inlineStr">
+      <c r="C219" t="inlineStr">
         <is>
           <t>conf/icse/SilveiraB11</t>
         </is>
       </c>
-      <c r="D214" t="inlineStr">
+      <c r="D219" t="inlineStr">
         <is>
           <t>A cloud-aware API for semi-structured BLOB databases addressing data overflow</t>
         </is>
       </c>
-      <c r="E214" t="inlineStr">
+      <c r="E219" t="inlineStr">
         <is>
           <t>db/conf/icse/topi2011.html#SilveiraB11</t>
         </is>
       </c>
-      <c r="F214" t="inlineStr">
+      <c r="F219" t="inlineStr">
         <is>
           <t>conf/icse/</t>
         </is>
       </c>
-      <c r="G214" t="n">
+      <c r="G219" t="n">
         <v>2011</v>
       </c>
-      <c r="H214" t="inlineStr">
+      <c r="H219" t="inlineStr">
         <is>
           <t>conf/icse/2011topi</t>
         </is>
       </c>
     </row>
-    <row r="215">
-      <c r="A215" t="inlineStr">
+    <row r="220">
+      <c r="A220" t="inlineStr">
         <is>
           <t>Barbara A. Kitchenham and Cat Kutay and D. Ross Jeffery and Colin Connaughton</t>
         </is>
       </c>
-      <c r="B215" t="inlineStr">
+      <c r="B220" t="inlineStr">
         <is>
           <t>@inproceedings{a.:2006,
 booktitle = {International Conference on Software Engineering (ICSE)}, 
@@ -9433,42 +9658,42 @@
 }</t>
         </is>
       </c>
-      <c r="C215" t="inlineStr">
+      <c r="C220" t="inlineStr">
         <is>
           <t>conf/icse/KitchenhamKJC06</t>
         </is>
       </c>
-      <c r="D215" t="inlineStr">
+      <c r="D220" t="inlineStr">
         <is>
           <t>Lessons learnt from the analysis of large-scale corporate databases</t>
         </is>
       </c>
-      <c r="E215" t="inlineStr">
+      <c r="E220" t="inlineStr">
         <is>
           <t>db/conf/icse/icse2006.html#KitchenhamKJC06</t>
         </is>
       </c>
-      <c r="F215" t="inlineStr">
+      <c r="F220" t="inlineStr">
         <is>
           <t>conf/icse/</t>
         </is>
       </c>
-      <c r="G215" t="n">
+      <c r="G220" t="n">
         <v>2006</v>
       </c>
-      <c r="H215" t="inlineStr">
+      <c r="H220" t="inlineStr">
         <is>
           <t>conf/icse/2006</t>
         </is>
       </c>
     </row>
-    <row r="216">
-      <c r="A216" t="inlineStr">
+    <row r="221">
+      <c r="A221" t="inlineStr">
         <is>
           <t>Carl Gould 0001 and Zhendong Su and Premkumar T. Devanbu</t>
         </is>
       </c>
-      <c r="B216" t="inlineStr">
+      <c r="B221" t="inlineStr">
         <is>
           <t>@inproceedings{gould:2004,
 booktitle = {International Conference on Software Engineering (ICSE)}, 
@@ -9478,42 +9703,42 @@
 }</t>
         </is>
       </c>
-      <c r="C216" t="inlineStr">
+      <c r="C221" t="inlineStr">
         <is>
           <t>conf/icse/GouldSD04</t>
         </is>
       </c>
-      <c r="D216" t="inlineStr">
+      <c r="D221" t="inlineStr">
         <is>
           <t>Static Checking of Dynamically Generated Queries in Database Applications</t>
         </is>
       </c>
-      <c r="E216" t="inlineStr">
+      <c r="E221" t="inlineStr">
         <is>
           <t>db/conf/icse/icse2004.html#GouldSD04</t>
         </is>
       </c>
-      <c r="F216" t="inlineStr">
+      <c r="F221" t="inlineStr">
         <is>
           <t>conf/icse/</t>
         </is>
       </c>
-      <c r="G216" t="n">
+      <c r="G221" t="n">
         <v>2004</v>
       </c>
-      <c r="H216" t="inlineStr">
+      <c r="H221" t="inlineStr">
         <is>
           <t>conf/icse/2004</t>
         </is>
       </c>
     </row>
-    <row r="217">
-      <c r="A217" t="inlineStr">
+    <row r="222">
+      <c r="A222" t="inlineStr">
         <is>
           <t>Lin Chiu and Ming T. Liu</t>
         </is>
       </c>
-      <c r="B217" t="inlineStr">
+      <c r="B222" t="inlineStr">
         <is>
           <t>@inproceedings{chiu:1988,
 booktitle = {International Conference on Software Engineering (ICSE)}, 
@@ -9523,42 +9748,42 @@
 }</t>
         </is>
       </c>
-      <c r="C217" t="inlineStr">
+      <c r="C222" t="inlineStr">
         <is>
           <t>conf/icse/ChiuL88</t>
         </is>
       </c>
-      <c r="D217" t="inlineStr">
+      <c r="D222" t="inlineStr">
         <is>
           <t>High-Level Specification of Concurrency Control in Distributed Database Systems</t>
         </is>
       </c>
-      <c r="E217" t="inlineStr">
+      <c r="E222" t="inlineStr">
         <is>
           <t>db/conf/icse/icse88.html#ChiuL88</t>
         </is>
       </c>
-      <c r="F217" t="inlineStr">
+      <c r="F222" t="inlineStr">
         <is>
           <t>conf/icse/</t>
         </is>
       </c>
-      <c r="G217" t="n">
+      <c r="G222" t="n">
         <v>1988</v>
       </c>
-      <c r="H217" t="inlineStr">
+      <c r="H222" t="inlineStr">
         <is>
           <t>conf/icse/1988</t>
         </is>
       </c>
     </row>
-    <row r="218">
-      <c r="A218" t="inlineStr">
+    <row r="223">
+      <c r="A223" t="inlineStr">
         <is>
           <t>Michael de Jong and Arie van Deursen and Anthony Cleve</t>
         </is>
       </c>
-      <c r="B218" t="inlineStr">
+      <c r="B223" t="inlineStr">
         <is>
           <t>@inproceedings{de:2017,
 booktitle = {International Conference on Software Engineering (ICSE)}, 
@@ -9568,42 +9793,42 @@
 }</t>
         </is>
       </c>
-      <c r="C218" t="inlineStr">
+      <c r="C223" t="inlineStr">
         <is>
           <t>conf/icse/JongDC17</t>
         </is>
       </c>
-      <c r="D218" t="inlineStr">
+      <c r="D223" t="inlineStr">
         <is>
           <t>Zero-Downtime SQL Database Schema Evolution for Continuous Deployment</t>
         </is>
       </c>
-      <c r="E218" t="inlineStr">
+      <c r="E223" t="inlineStr">
         <is>
           <t>db/conf/icse/icse2017seip.html#JongDC17</t>
         </is>
       </c>
-      <c r="F218" t="inlineStr">
+      <c r="F223" t="inlineStr">
         <is>
           <t>conf/icse/</t>
         </is>
       </c>
-      <c r="G218" t="n">
+      <c r="G223" t="n">
         <v>2017</v>
       </c>
-      <c r="H218" t="inlineStr">
+      <c r="H223" t="inlineStr">
         <is>
           <t>conf/icse/2017seip</t>
         </is>
       </c>
     </row>
-    <row r="219">
-      <c r="A219" t="inlineStr">
+    <row r="224">
+      <c r="A224" t="inlineStr">
         <is>
           <t>Yuan Tian 0008 and David Lo 0001 and Julia L. Lawall</t>
         </is>
       </c>
-      <c r="B219" t="inlineStr">
+      <c r="B224" t="inlineStr">
         <is>
           <t>@inproceedings{tian:2014,
 booktitle = {International Conference on Software Engineering (ICSE)}, 
@@ -9613,42 +9838,42 @@
 }</t>
         </is>
       </c>
-      <c r="C219" t="inlineStr">
+      <c r="C224" t="inlineStr">
         <is>
           <t>conf/icse/TianLL14</t>
         </is>
       </c>
-      <c r="D219" t="inlineStr">
+      <c r="D224" t="inlineStr">
         <is>
           <t>SEWordSim: software-specific word similarity database</t>
         </is>
       </c>
-      <c r="E219" t="inlineStr">
+      <c r="E224" t="inlineStr">
         <is>
           <t>db/conf/icse/icse2014c.html#TianLL14</t>
         </is>
       </c>
-      <c r="F219" t="inlineStr">
+      <c r="F224" t="inlineStr">
         <is>
           <t>conf/icse/</t>
         </is>
       </c>
-      <c r="G219" t="n">
+      <c r="G224" t="n">
         <v>2014</v>
       </c>
-      <c r="H219" t="inlineStr">
+      <c r="H224" t="inlineStr">
         <is>
           <t>conf/icse/2014c</t>
         </is>
       </c>
     </row>
-    <row r="220">
-      <c r="A220" t="inlineStr">
+    <row r="225">
+      <c r="A225" t="inlineStr">
         <is>
           <t>Oskari Koskimies and Johan Wikman and Tapani Mikola and Antero Taivalsaari</t>
         </is>
       </c>
-      <c r="B220" t="inlineStr">
+      <c r="B225" t="inlineStr">
         <is>
           <t>@inproceedings{koskimies:2015,
 booktitle = {International Conference on Software Engineering (ICSE)}, 
@@ -9658,42 +9883,42 @@
 }</t>
         </is>
       </c>
-      <c r="C220" t="inlineStr">
+      <c r="C225" t="inlineStr">
         <is>
           <t>conf/icse/KoskimiesWMT15</t>
         </is>
       </c>
-      <c r="D220" t="inlineStr">
+      <c r="D225" t="inlineStr">
         <is>
           <t>EDB: A Multi-master Database for Liquid Multi-device Software</t>
         </is>
       </c>
-      <c r="E220" t="inlineStr">
+      <c r="E225" t="inlineStr">
         <is>
           <t>db/conf/icse/mobilesoft2015.html#KoskimiesWMT15</t>
         </is>
       </c>
-      <c r="F220" t="inlineStr">
+      <c r="F225" t="inlineStr">
         <is>
           <t>conf/icse/</t>
         </is>
       </c>
-      <c r="G220" t="n">
+      <c r="G225" t="n">
         <v>2015</v>
       </c>
-      <c r="H220" t="inlineStr">
+      <c r="H225" t="inlineStr">
         <is>
           <t>conf/icse/2015mobilesoft</t>
         </is>
       </c>
     </row>
-    <row r="221">
-      <c r="A221" t="inlineStr">
+    <row r="226">
+      <c r="A226" t="inlineStr">
         <is>
           <t>Claudio de la Riva and María José Suárez Cabal and Javier Tuya</t>
         </is>
       </c>
-      <c r="B221" t="inlineStr">
+      <c r="B226" t="inlineStr">
         <is>
           <t>@inproceedings{de:2010,
 booktitle = {International Conference on Software Engineering (ICSE)}, 
@@ -9703,42 +9928,42 @@
 }</t>
         </is>
       </c>
-      <c r="C221" t="inlineStr">
+      <c r="C226" t="inlineStr">
         <is>
           <t>conf/icse/RivaCT10</t>
         </is>
       </c>
-      <c r="D221" t="inlineStr">
+      <c r="D226" t="inlineStr">
         <is>
           <t>Constraint-based test database generation for SQL queries</t>
         </is>
       </c>
-      <c r="E221" t="inlineStr">
+      <c r="E226" t="inlineStr">
         <is>
           <t>db/conf/icse/ast2010.html#RivaCT10</t>
         </is>
       </c>
-      <c r="F221" t="inlineStr">
+      <c r="F226" t="inlineStr">
         <is>
           <t>conf/icse/</t>
         </is>
       </c>
-      <c r="G221" t="n">
+      <c r="G226" t="n">
         <v>2010</v>
       </c>
-      <c r="H221" t="inlineStr">
+      <c r="H226" t="inlineStr">
         <is>
           <t>conf/icse/2010ast</t>
         </is>
       </c>
     </row>
-    <row r="222">
-      <c r="A222" t="inlineStr">
+    <row r="227">
+      <c r="A227" t="inlineStr">
         <is>
           <t>Nate Kube and Kevin Yoo and Daniel Hoffman</t>
         </is>
       </c>
-      <c r="B222" t="inlineStr">
+      <c r="B227" t="inlineStr">
         <is>
           <t>@inproceedings{kube:2011,
 booktitle = {International Conference on Software Engineering (ICSE)}, 
@@ -9748,42 +9973,42 @@
 }</t>
         </is>
       </c>
-      <c r="C222" t="inlineStr">
+      <c r="C227" t="inlineStr">
         <is>
           <t>conf/icse/KubeYH11</t>
         </is>
       </c>
-      <c r="D222" t="inlineStr">
+      <c r="D227" t="inlineStr">
         <is>
           <t>Automated testing of industrial control devices: the delphi database</t>
         </is>
       </c>
-      <c r="E222" t="inlineStr">
+      <c r="E227" t="inlineStr">
         <is>
           <t>db/conf/icse/ast2011.html#KubeYH11</t>
         </is>
       </c>
-      <c r="F222" t="inlineStr">
+      <c r="F227" t="inlineStr">
         <is>
           <t>conf/icse/</t>
         </is>
       </c>
-      <c r="G222" t="n">
+      <c r="G227" t="n">
         <v>2011</v>
       </c>
-      <c r="H222" t="inlineStr">
+      <c r="H227" t="inlineStr">
         <is>
           <t>conf/icse/2011ast</t>
         </is>
       </c>
     </row>
-    <row r="223">
-      <c r="A223" t="inlineStr">
+    <row r="228">
+      <c r="A228" t="inlineStr">
         <is>
           <t>Percy E. Salas and Edgard Marx and Alexander Mera and José Viterbo</t>
         </is>
       </c>
-      <c r="B223" t="inlineStr">
+      <c r="B228" t="inlineStr">
         <is>
           <t>@inproceedings{e.:2011,
 booktitle = {International Conference on Software Engineering (ICSE)}, 
@@ -9793,42 +10018,42 @@
 }</t>
         </is>
       </c>
-      <c r="C223" t="inlineStr">
+      <c r="C228" t="inlineStr">
         <is>
           <t>conf/icse/SalasMMV11</t>
         </is>
       </c>
-      <c r="D223" t="inlineStr">
+      <c r="D228" t="inlineStr">
         <is>
           <t>RDB2RDF plugin: relational databases to RDF plugin for eclipse</t>
         </is>
       </c>
-      <c r="E223" t="inlineStr">
+      <c r="E228" t="inlineStr">
         <is>
           <t>db/conf/icse/topi2011.html#SalasMMV11</t>
         </is>
       </c>
-      <c r="F223" t="inlineStr">
+      <c r="F228" t="inlineStr">
         <is>
           <t>conf/icse/</t>
         </is>
       </c>
-      <c r="G223" t="n">
+      <c r="G228" t="n">
         <v>2011</v>
       </c>
-      <c r="H223" t="inlineStr">
+      <c r="H228" t="inlineStr">
         <is>
           <t>conf/icse/2011topi</t>
         </is>
       </c>
     </row>
-    <row r="224">
-      <c r="A224" t="inlineStr">
+    <row r="229">
+      <c r="A229" t="inlineStr">
         <is>
           <t>Tushar Sharma and Marios Fragkoulis and Stamatia Rizou and Magiel Bruntink and Diomidis Spinellis</t>
         </is>
       </c>
-      <c r="B224" t="inlineStr">
+      <c r="B229" t="inlineStr">
         <is>
           <t>@inproceedings{sharma:2018,
 booktitle = {International Conference on Software Engineering (ICSE)}, 
@@ -9838,42 +10063,42 @@
 }</t>
         </is>
       </c>
-      <c r="C224" t="inlineStr">
+      <c r="C229" t="inlineStr">
         <is>
           <t>conf/icse/SharmaFRBS18</t>
         </is>
       </c>
-      <c r="D224" t="inlineStr">
+      <c r="D229" t="inlineStr">
         <is>
           <t>Smelly relations: measuring and understanding database schema quality</t>
         </is>
       </c>
-      <c r="E224" t="inlineStr">
+      <c r="E229" t="inlineStr">
         <is>
           <t>db/conf/icse/seip2018.html#SharmaFRBS18</t>
         </is>
       </c>
-      <c r="F224" t="inlineStr">
+      <c r="F229" t="inlineStr">
         <is>
           <t>conf/icse/</t>
         </is>
       </c>
-      <c r="G224" t="n">
+      <c r="G229" t="n">
         <v>2018</v>
       </c>
-      <c r="H224" t="inlineStr">
+      <c r="H229" t="inlineStr">
         <is>
           <t>conf/icse/2018seip</t>
         </is>
       </c>
     </row>
-    <row r="225">
-      <c r="A225" t="inlineStr">
+    <row r="230">
+      <c r="A230" t="inlineStr">
         <is>
           <t>Junwen Yang and Cong Yan and Chengcheng Wan and Shan Lu and Alvin Cheung</t>
         </is>
       </c>
-      <c r="B225" t="inlineStr">
+      <c r="B230" t="inlineStr">
         <is>
           <t>@inproceedings{yang:2019,
 booktitle = {International Conference on Software Engineering (ICSE)}, 
@@ -9883,42 +10108,42 @@
 }</t>
         </is>
       </c>
-      <c r="C225" t="inlineStr">
+      <c r="C230" t="inlineStr">
         <is>
           <t>conf/icse/YangYWLC19</t>
         </is>
       </c>
-      <c r="D225" t="inlineStr">
+      <c r="D230" t="inlineStr">
         <is>
           <t>View-centric performance optimization for database-backed web applications</t>
         </is>
       </c>
-      <c r="E225" t="inlineStr">
+      <c r="E230" t="inlineStr">
         <is>
           <t>db/conf/icse/icse2019.html#YangYWLC19</t>
         </is>
       </c>
-      <c r="F225" t="inlineStr">
+      <c r="F230" t="inlineStr">
         <is>
           <t>conf/icse/</t>
         </is>
       </c>
-      <c r="G225" t="n">
+      <c r="G230" t="n">
         <v>2019</v>
       </c>
-      <c r="H225" t="inlineStr">
+      <c r="H230" t="inlineStr">
         <is>
           <t>conf/icse/2019</t>
         </is>
       </c>
     </row>
-    <row r="226">
-      <c r="A226" t="inlineStr">
+    <row r="231">
+      <c r="A231" t="inlineStr">
         <is>
           <t>Csaba Nagy and Anthony Cleve</t>
         </is>
       </c>
-      <c r="B226" t="inlineStr">
+      <c r="B231" t="inlineStr">
         <is>
           <t>@inproceedings{nagy:2018,
 booktitle = {International Conference on Software Engineering (ICSE)}, 
@@ -9928,42 +10153,42 @@
 }</t>
         </is>
       </c>
-      <c r="C226" t="inlineStr">
+      <c r="C231" t="inlineStr">
         <is>
           <t>conf/icse/NagyC18</t>
         </is>
       </c>
-      <c r="D226" t="inlineStr">
+      <c r="D231" t="inlineStr">
         <is>
           <t>SQLInspect: a static analyzer to inspect database usage in Java applications</t>
         </is>
       </c>
-      <c r="E226" t="inlineStr">
+      <c r="E231" t="inlineStr">
         <is>
           <t>db/conf/icse/icse2018c.html#NagyC18</t>
         </is>
       </c>
-      <c r="F226" t="inlineStr">
+      <c r="F231" t="inlineStr">
         <is>
           <t>conf/icse/</t>
         </is>
       </c>
-      <c r="G226" t="n">
+      <c r="G231" t="n">
         <v>2018</v>
       </c>
-      <c r="H226" t="inlineStr">
+      <c r="H231" t="inlineStr">
         <is>
           <t>conf/icse/2018c</t>
         </is>
       </c>
     </row>
-    <row r="227">
-      <c r="A227" t="inlineStr">
+    <row r="232">
+      <c r="A232" t="inlineStr">
         <is>
           <t>Michael de Jong and Arie van Deursen</t>
         </is>
       </c>
-      <c r="B227" t="inlineStr">
+      <c r="B232" t="inlineStr">
         <is>
           <t>@inproceedings{de:2015,
 booktitle = {International Conference on Software Engineering (ICSE)}, 
@@ -9973,42 +10198,42 @@
 }</t>
         </is>
       </c>
-      <c r="C227" t="inlineStr">
+      <c r="C232" t="inlineStr">
         <is>
           <t>conf/icse/JongD15</t>
         </is>
       </c>
-      <c r="D227" t="inlineStr">
+      <c r="D232" t="inlineStr">
         <is>
           <t>Continuous Deployment and Schema Evolution in SQL Databases</t>
         </is>
       </c>
-      <c r="E227" t="inlineStr">
+      <c r="E232" t="inlineStr">
         <is>
           <t>db/conf/icse/releng2015.html#JongD15</t>
         </is>
       </c>
-      <c r="F227" t="inlineStr">
+      <c r="F232" t="inlineStr">
         <is>
           <t>conf/icse/</t>
         </is>
       </c>
-      <c r="G227" t="n">
+      <c r="G232" t="n">
         <v>2015</v>
       </c>
-      <c r="H227" t="inlineStr">
+      <c r="H232" t="inlineStr">
         <is>
           <t>conf/icse/2015releng</t>
         </is>
       </c>
     </row>
-    <row r="228">
-      <c r="A228" t="inlineStr">
+    <row r="233">
+      <c r="A233" t="inlineStr">
         <is>
           <t>Ramkrishna Chatterjee and Gopalan Arun and Sanjay Agarwal and Ben Speckhard and Ramesh Vasudevan</t>
         </is>
       </c>
-      <c r="B228" t="inlineStr">
+      <c r="B233" t="inlineStr">
         <is>
           <t>@inproceedings{chatterjee:2004,
 booktitle = {International Conference on Software Engineering (ICSE)}, 
@@ -10018,42 +10243,42 @@
 }</t>
         </is>
       </c>
-      <c r="C228" t="inlineStr">
+      <c r="C233" t="inlineStr">
         <is>
           <t>conf/icse/ChatterjeeAASV04</t>
         </is>
       </c>
-      <c r="D228" t="inlineStr">
+      <c r="D233" t="inlineStr">
         <is>
           <t>Using Data Versioning in Database Application Development</t>
         </is>
       </c>
-      <c r="E228" t="inlineStr">
+      <c r="E233" t="inlineStr">
         <is>
           <t>db/conf/icse/icse2004.html#ChatterjeeAASV04</t>
         </is>
       </c>
-      <c r="F228" t="inlineStr">
+      <c r="F233" t="inlineStr">
         <is>
           <t>conf/icse/</t>
         </is>
       </c>
-      <c r="G228" t="n">
+      <c r="G233" t="n">
         <v>2004</v>
       </c>
-      <c r="H228" t="inlineStr">
+      <c r="H233" t="inlineStr">
         <is>
           <t>conf/icse/2004</t>
         </is>
       </c>
     </row>
-    <row r="229">
-      <c r="A229" t="inlineStr">
+    <row r="234">
+      <c r="A234" t="inlineStr">
         <is>
           <t>Phil McMinn and Gregory M. Kapfhammer and Chris J. Wright</t>
         </is>
       </c>
-      <c r="B229" t="inlineStr">
+      <c r="B234" t="inlineStr">
         <is>
           <t>@inproceedings{mcminn:2016,
 booktitle = {International Conference on Software Engineering (ICSE)}, 
@@ -10063,42 +10288,42 @@
 }</t>
         </is>
       </c>
-      <c r="C229" t="inlineStr">
+      <c r="C234" t="inlineStr">
         <is>
           <t>conf/icse/McMinnKW16</t>
         </is>
       </c>
-      <c r="D229" t="inlineStr">
+      <c r="D234" t="inlineStr">
         <is>
           <t>Virtual mutation analysis of relational database schemas</t>
         </is>
       </c>
-      <c r="E229" t="inlineStr">
+      <c r="E234" t="inlineStr">
         <is>
           <t>db/conf/icse/ast2016.html#McMinnKW16</t>
         </is>
       </c>
-      <c r="F229" t="inlineStr">
+      <c r="F234" t="inlineStr">
         <is>
           <t>conf/icse/</t>
         </is>
       </c>
-      <c r="G229" t="n">
+      <c r="G234" t="n">
         <v>2016</v>
       </c>
-      <c r="H229" t="inlineStr">
+      <c r="H234" t="inlineStr">
         <is>
           <t>conf/icse/2016ast</t>
         </is>
       </c>
     </row>
-    <row r="230">
-      <c r="A230" t="inlineStr">
+    <row r="235">
+      <c r="A235" t="inlineStr">
         <is>
           <t>Junwen Yang and Pranav Subramaniam and Shan Lu and Cong Yan and Alvin Cheung</t>
         </is>
       </c>
-      <c r="B230" t="inlineStr">
+      <c r="B235" t="inlineStr">
         <is>
           <t>@inproceedings{yang:2018,
 booktitle = {International Conference on Software Engineering (ICSE)}, 
@@ -10108,42 +10333,42 @@
 }</t>
         </is>
       </c>
-      <c r="C230" t="inlineStr">
+      <c r="C235" t="inlineStr">
         <is>
           <t>conf/icse/YangSLYC18</t>
         </is>
       </c>
-      <c r="D230" t="inlineStr">
+      <c r="D235" t="inlineStr">
         <is>
           <t>How not to structure your database-backed web applications: a study of performance bugs in the wild</t>
         </is>
       </c>
-      <c r="E230" t="inlineStr">
+      <c r="E235" t="inlineStr">
         <is>
           <t>db/conf/icse/icse2018.html#YangSLYC18</t>
         </is>
       </c>
-      <c r="F230" t="inlineStr">
+      <c r="F235" t="inlineStr">
         <is>
           <t>conf/icse/</t>
         </is>
       </c>
-      <c r="G230" t="n">
+      <c r="G235" t="n">
         <v>2018</v>
       </c>
-      <c r="H230" t="inlineStr">
+      <c r="H235" t="inlineStr">
         <is>
           <t>conf/icse/2018</t>
         </is>
       </c>
     </row>
-    <row r="231">
-      <c r="A231" t="inlineStr">
+    <row r="236">
+      <c r="A236" t="inlineStr">
         <is>
           <t>Jesús M. González-Barahona and Gregorio Robles and Daniel Izquierdo-Cortazar</t>
         </is>
       </c>
-      <c r="B231" t="inlineStr">
+      <c r="B236" t="inlineStr">
         <is>
           <t>@inproceedings{m.:2015,
 booktitle = {International Conference on Mining Software Repositories (MSR)}, 
@@ -10153,42 +10378,42 @@
 }</t>
         </is>
       </c>
-      <c r="C231" t="inlineStr">
+      <c r="C236" t="inlineStr">
         <is>
           <t>conf/msr/Gonzalez-Barahona15</t>
         </is>
       </c>
-      <c r="D231" t="inlineStr">
+      <c r="D236" t="inlineStr">
         <is>
           <t>The MetricsGrimoire Database Collection</t>
         </is>
       </c>
-      <c r="E231" t="inlineStr">
+      <c r="E236" t="inlineStr">
         <is>
           <t>db/conf/msr/msr2015.html#Gonzalez-Barahona15</t>
         </is>
       </c>
-      <c r="F231" t="inlineStr">
+      <c r="F236" t="inlineStr">
         <is>
           <t>conf/msr/</t>
         </is>
       </c>
-      <c r="G231" t="n">
+      <c r="G236" t="n">
         <v>2015</v>
       </c>
-      <c r="H231" t="inlineStr">
+      <c r="H236" t="inlineStr">
         <is>
           <t>conf/msr/2015</t>
         </is>
       </c>
     </row>
-    <row r="232">
-      <c r="A232" t="inlineStr">
+    <row r="237">
+      <c r="A237" t="inlineStr">
         <is>
           <t>Omar Alonso and Premkumar T. Devanbu and Michael Gertz</t>
         </is>
       </c>
-      <c r="B232" t="inlineStr">
+      <c r="B237" t="inlineStr">
         <is>
           <t>@inproceedings{alonso:2004,
 booktitle = {International Conference on Mining Software Repositories (MSR)}, 
@@ -10198,42 +10423,42 @@
 }</t>
         </is>
       </c>
-      <c r="C232" t="inlineStr">
+      <c r="C237" t="inlineStr">
         <is>
           <t>conf/msr/AlonsoDG04</t>
         </is>
       </c>
-      <c r="D232" t="inlineStr">
+      <c r="D237" t="inlineStr">
         <is>
           <t>Database Techniques for the Analysis and Exploration of Software Repositories</t>
         </is>
       </c>
-      <c r="E232" t="inlineStr">
+      <c r="E237" t="inlineStr">
         <is>
           <t>db/conf/msr/msr2004.html#AlonsoDG04</t>
         </is>
       </c>
-      <c r="F232" t="inlineStr">
+      <c r="F237" t="inlineStr">
         <is>
           <t>conf/msr/</t>
         </is>
       </c>
-      <c r="G232" t="n">
+      <c r="G237" t="n">
         <v>2004</v>
       </c>
-      <c r="H232" t="inlineStr">
+      <c r="H237" t="inlineStr">
         <is>
           <t>conf/msr/2004</t>
         </is>
       </c>
     </row>
-    <row r="233">
-      <c r="A233" t="inlineStr">
+    <row r="238">
+      <c r="A238" t="inlineStr">
         <is>
           <t>Alexander Breckel</t>
         </is>
       </c>
-      <c r="B233" t="inlineStr">
+      <c r="B238" t="inlineStr">
         <is>
           <t>@inproceedings{breckel:2012,
 booktitle = {International Conference on Mining Software Repositories (MSR)}, 
@@ -10243,42 +10468,42 @@
 }</t>
         </is>
       </c>
-      <c r="C233" t="inlineStr">
+      <c r="C238" t="inlineStr">
         <is>
           <t>conf/msr/Breckel12</t>
         </is>
       </c>
-      <c r="D233" t="inlineStr">
+      <c r="D238" t="inlineStr">
         <is>
           <t>Error mining: Bug detection through comparison with large code databases</t>
         </is>
       </c>
-      <c r="E233" t="inlineStr">
+      <c r="E238" t="inlineStr">
         <is>
           <t>db/conf/msr/msr2012.html#Breckel12</t>
         </is>
       </c>
-      <c r="F233" t="inlineStr">
+      <c r="F238" t="inlineStr">
         <is>
           <t>conf/msr/</t>
         </is>
       </c>
-      <c r="G233" t="n">
+      <c r="G238" t="n">
         <v>2012</v>
       </c>
-      <c r="H233" t="inlineStr">
+      <c r="H238" t="inlineStr">
         <is>
           <t>conf/msr/2012</t>
         </is>
       </c>
     </row>
-    <row r="234">
-      <c r="A234" t="inlineStr">
+    <row r="239">
+      <c r="A239" t="inlineStr">
         <is>
           <t>Remco Bloemen and Chintan Amrit and Stefan Kuhlmann and Gonzalo Ordóñez-Matamoros</t>
         </is>
       </c>
-      <c r="B234" t="inlineStr">
+      <c r="B239" t="inlineStr">
         <is>
           <t>@inproceedings{bloemen:2014,
 booktitle = {International Conference on Mining Software Repositories (MSR)}, 
@@ -10288,42 +10513,42 @@
 }</t>
         </is>
       </c>
-      <c r="C234" t="inlineStr">
+      <c r="C239" t="inlineStr">
         <is>
           <t>conf/msr/BloemenAKO14</t>
         </is>
       </c>
-      <c r="D234" t="inlineStr">
+      <c r="D239" t="inlineStr">
         <is>
           <t>Innovation diffusion in open source software: preliminary analysis of dependency changes in the gentoo portage package database</t>
         </is>
       </c>
-      <c r="E234" t="inlineStr">
+      <c r="E239" t="inlineStr">
         <is>
           <t>db/conf/msr/msr2014.html#BloemenAKO14</t>
         </is>
       </c>
-      <c r="F234" t="inlineStr">
+      <c r="F239" t="inlineStr">
         <is>
           <t>conf/msr/</t>
         </is>
       </c>
-      <c r="G234" t="n">
+      <c r="G239" t="n">
         <v>2014</v>
       </c>
-      <c r="H234" t="inlineStr">
+      <c r="H239" t="inlineStr">
         <is>
           <t>conf/msr/2014</t>
         </is>
       </c>
     </row>
-    <row r="235">
-      <c r="A235" t="inlineStr">
+    <row r="240">
+      <c r="A240" t="inlineStr">
         <is>
           <t>Lucas Nussbaum and Stefano Zacchiroli</t>
         </is>
       </c>
-      <c r="B235" t="inlineStr">
+      <c r="B240" t="inlineStr">
         <is>
           <t>@inproceedings{nussbaum:2010,
 booktitle = {International Conference on Mining Software Repositories (MSR)}, 
@@ -10333,42 +10558,42 @@
 }</t>
         </is>
       </c>
-      <c r="C235" t="inlineStr">
+      <c r="C240" t="inlineStr">
         <is>
           <t>conf/msr/NussbaumZ10</t>
         </is>
       </c>
-      <c r="D235" t="inlineStr">
+      <c r="D240" t="inlineStr">
         <is>
           <t>The Ultimate Debian Database: Consolidating bazaar metadata for Quality Assurance and data mining</t>
         </is>
       </c>
-      <c r="E235" t="inlineStr">
+      <c r="E240" t="inlineStr">
         <is>
           <t>db/conf/msr/msr2010.html#NussbaumZ10</t>
         </is>
       </c>
-      <c r="F235" t="inlineStr">
+      <c r="F240" t="inlineStr">
         <is>
           <t>conf/msr/</t>
         </is>
       </c>
-      <c r="G235" t="n">
+      <c r="G240" t="n">
         <v>2010</v>
       </c>
-      <c r="H235" t="inlineStr">
+      <c r="H240" t="inlineStr">
         <is>
           <t>conf/msr/2010</t>
         </is>
       </c>
     </row>
-    <row r="236">
-      <c r="A236" t="inlineStr">
+    <row r="241">
+      <c r="A241" t="inlineStr">
         <is>
           <t>Mashel Al-Barak and Rami Bahsoon</t>
         </is>
       </c>
-      <c r="B236" t="inlineStr">
+      <c r="B241" t="inlineStr">
         <is>
           <t>@inproceedings{al-barak:2016,
 booktitle = {International Conference on Software Maintenance and Evolution (ICSME)}, 
@@ -10378,42 +10603,42 @@
 }</t>
         </is>
       </c>
-      <c r="C236" t="inlineStr">
+      <c r="C241" t="inlineStr">
         <is>
           <t>conf/icsm/Al-BarakB16</t>
         </is>
       </c>
-      <c r="D236" t="inlineStr">
+      <c r="D241" t="inlineStr">
         <is>
           <t>Database Design Debts through Examining Schema Evolution</t>
         </is>
       </c>
-      <c r="E236" t="inlineStr">
+      <c r="E241" t="inlineStr">
         <is>
           <t>db/conf/icsm/mtd2016.html#Al-BarakB16</t>
         </is>
       </c>
-      <c r="F236" t="inlineStr">
+      <c r="F241" t="inlineStr">
         <is>
           <t>conf/icsm/</t>
         </is>
       </c>
-      <c r="G236" t="n">
+      <c r="G241" t="n">
         <v>2016</v>
       </c>
-      <c r="H236" t="inlineStr">
+      <c r="H241" t="inlineStr">
         <is>
           <t>conf/icsm/2016mtd</t>
         </is>
       </c>
     </row>
-    <row r="237">
-      <c r="A237" t="inlineStr">
+    <row r="242">
+      <c r="A242" t="inlineStr">
         <is>
           <t>Mathieu Goeminne and Tom Mens</t>
         </is>
       </c>
-      <c r="B237" t="inlineStr">
+      <c r="B242" t="inlineStr">
         <is>
           <t>@inproceedings{goeminne:2015,
 booktitle = {International Conference on Software Maintenance and Evolution (ICSME)}, 
@@ -10423,42 +10648,42 @@
 }</t>
         </is>
       </c>
-      <c r="C237" t="inlineStr">
+      <c r="C242" t="inlineStr">
         <is>
           <t>conf/icsm/GoeminneM15</t>
         </is>
       </c>
-      <c r="D237" t="inlineStr">
+      <c r="D242" t="inlineStr">
         <is>
           <t>Towards a survival analysis of database framework usage in Java projects</t>
         </is>
       </c>
-      <c r="E237" t="inlineStr">
+      <c r="E242" t="inlineStr">
         <is>
           <t>db/conf/icsm/icsme2015.html#GoeminneM15</t>
         </is>
       </c>
-      <c r="F237" t="inlineStr">
+      <c r="F242" t="inlineStr">
         <is>
           <t>conf/icsm/</t>
         </is>
       </c>
-      <c r="G237" t="n">
+      <c r="G242" t="n">
         <v>2015</v>
       </c>
-      <c r="H237" t="inlineStr">
+      <c r="H242" t="inlineStr">
         <is>
           <t>conf/icsm/2015</t>
         </is>
       </c>
     </row>
-    <row r="238">
-      <c r="A238" t="inlineStr">
+    <row r="243">
+      <c r="A243" t="inlineStr">
         <is>
           <t>Jens H. Jahnke and Wilhelm Schäfer and Albert Zündorf</t>
         </is>
       </c>
-      <c r="B238" t="inlineStr">
+      <c r="B243" t="inlineStr">
         <is>
           <t>@inproceedings{h.:1996,
 booktitle = {International Conference on Software Maintenance and Evolution (ICSME)}, 
@@ -10468,42 +10693,42 @@
 }</t>
         </is>
       </c>
-      <c r="C238" t="inlineStr">
+      <c r="C243" t="inlineStr">
         <is>
           <t>conf/icsm/JahnkeSZ96</t>
         </is>
       </c>
-      <c r="D238" t="inlineStr">
+      <c r="D243" t="inlineStr">
         <is>
           <t>A Design Environment for Migrating Relational to Object Oriented Database Systems</t>
         </is>
       </c>
-      <c r="E238" t="inlineStr">
+      <c r="E243" t="inlineStr">
         <is>
           <t>db/conf/icsm/icsm1996.html#JahnkeSZ96</t>
         </is>
       </c>
-      <c r="F238" t="inlineStr">
+      <c r="F243" t="inlineStr">
         <is>
           <t>conf/icsm/</t>
         </is>
       </c>
-      <c r="G238" t="n">
+      <c r="G243" t="n">
         <v>1996</v>
       </c>
-      <c r="H238" t="inlineStr">
+      <c r="H243" t="inlineStr">
         <is>
           <t>conf/icsm/1996</t>
         </is>
       </c>
     </row>
-    <row r="239">
-      <c r="A239" t="inlineStr">
+    <row r="244">
+      <c r="A244" t="inlineStr">
         <is>
           <t>Jens H. Weber and Anthony Cleve and Loup Meurice and Francisco Javier Bermudez Ruiz</t>
         </is>
       </c>
-      <c r="B239" t="inlineStr">
+      <c r="B244" t="inlineStr">
         <is>
           <t>@inproceedings{h.:2014,
 booktitle = {International Conference on Software Maintenance and Evolution (ICSME)}, 
@@ -10513,42 +10738,42 @@
 }</t>
         </is>
       </c>
-      <c r="C239" t="inlineStr">
+      <c r="C244" t="inlineStr">
         <is>
           <t>conf/icsm/WeberCMR14</t>
         </is>
       </c>
-      <c r="D239" t="inlineStr">
+      <c r="D244" t="inlineStr">
         <is>
           <t>Managing Technical Debt in Database Schemas of Critical Software</t>
         </is>
       </c>
-      <c r="E239" t="inlineStr">
+      <c r="E244" t="inlineStr">
         <is>
           <t>db/conf/icsm/mtd2014.html#WeberCMR14</t>
         </is>
       </c>
-      <c r="F239" t="inlineStr">
+      <c r="F244" t="inlineStr">
         <is>
           <t>conf/icsm/</t>
         </is>
       </c>
-      <c r="G239" t="n">
+      <c r="G244" t="n">
         <v>2014</v>
       </c>
-      <c r="H239" t="inlineStr">
+      <c r="H244" t="inlineStr">
         <is>
           <t>conf/icsm/2014mtd</t>
         </is>
       </c>
     </row>
-    <row r="240">
-      <c r="A240" t="inlineStr">
+    <row r="245">
+      <c r="A245" t="inlineStr">
         <is>
           <t>Karla Saur and Tudor Dumitras and Michael W. Hicks</t>
         </is>
       </c>
-      <c r="B240" t="inlineStr">
+      <c r="B245" t="inlineStr">
         <is>
           <t>@inproceedings{saur:2016,
 booktitle = {International Conference on Software Maintenance and Evolution (ICSME)}, 
@@ -10558,42 +10783,42 @@
 }</t>
         </is>
       </c>
-      <c r="C240" t="inlineStr">
+      <c r="C245" t="inlineStr">
         <is>
           <t>conf/icsm/SaurDH16</t>
         </is>
       </c>
-      <c r="D240" t="inlineStr">
+      <c r="D245" t="inlineStr">
         <is>
           <t>Evolving NoSQL Databases without Downtime</t>
         </is>
       </c>
-      <c r="E240" t="inlineStr">
+      <c r="E245" t="inlineStr">
         <is>
           <t>db/conf/icsm/icsme2016.html#SaurDH16</t>
         </is>
       </c>
-      <c r="F240" t="inlineStr">
+      <c r="F245" t="inlineStr">
         <is>
           <t>conf/icsm/</t>
         </is>
       </c>
-      <c r="G240" t="n">
+      <c r="G245" t="n">
         <v>2016</v>
       </c>
-      <c r="H240" t="inlineStr">
+      <c r="H245" t="inlineStr">
         <is>
           <t>conf/icsm/2016</t>
         </is>
       </c>
     </row>
-    <row r="241">
-      <c r="A241" t="inlineStr">
+    <row r="246">
+      <c r="A246" t="inlineStr">
         <is>
           <t>Julien Delplanque and Anne Etien and Nicolas Anquetil and Olivier Auverlot</t>
         </is>
       </c>
-      <c r="B241" t="inlineStr">
+      <c r="B246" t="inlineStr">
         <is>
           <t>@inproceedings{delplanque:2018,
 booktitle = {International Conference on Software Maintenance and Evolution (ICSME)}, 
@@ -10603,42 +10828,42 @@
 }</t>
         </is>
       </c>
-      <c r="C241" t="inlineStr">
+      <c r="C246" t="inlineStr">
         <is>
           <t>conf/icsm/DelplanqueEAA18</t>
         </is>
       </c>
-      <c r="D241" t="inlineStr">
+      <c r="D246" t="inlineStr">
         <is>
           <t>Relational Database Schema Evolution: An Industrial Case Study</t>
         </is>
       </c>
-      <c r="E241" t="inlineStr">
+      <c r="E246" t="inlineStr">
         <is>
           <t>db/conf/icsm/icsme2018.html#DelplanqueEAA18</t>
         </is>
       </c>
-      <c r="F241" t="inlineStr">
+      <c r="F246" t="inlineStr">
         <is>
           <t>conf/icsm/</t>
         </is>
       </c>
-      <c r="G241" t="n">
+      <c r="G246" t="n">
         <v>2018</v>
       </c>
-      <c r="H241" t="inlineStr">
+      <c r="H246" t="inlineStr">
         <is>
           <t>conf/icsm/2018</t>
         </is>
       </c>
     </row>
-    <row r="242">
-      <c r="A242" t="inlineStr">
+    <row r="247">
+      <c r="A247" t="inlineStr">
         <is>
           <t>David Willmor and Suzanne M. Embury and Jianhua Shao 0001</t>
         </is>
       </c>
-      <c r="B242" t="inlineStr">
+      <c r="B247" t="inlineStr">
         <is>
           <t>@inproceedings{willmor:2004,
 booktitle = {International Conference on Software Maintenance and Evolution (ICSME)}, 
@@ -10648,42 +10873,42 @@
 }</t>
         </is>
       </c>
-      <c r="C242" t="inlineStr">
+      <c r="C247" t="inlineStr">
         <is>
           <t>conf/icsm/WillmorES04</t>
         </is>
       </c>
-      <c r="D242" t="inlineStr">
+      <c r="D247" t="inlineStr">
         <is>
           <t>Program Slicing in the Presence of a Database State</t>
         </is>
       </c>
-      <c r="E242" t="inlineStr">
+      <c r="E247" t="inlineStr">
         <is>
           <t>db/conf/icsm/icsm2004.html#WillmorES04</t>
         </is>
       </c>
-      <c r="F242" t="inlineStr">
+      <c r="F247" t="inlineStr">
         <is>
           <t>conf/icsm/</t>
         </is>
       </c>
-      <c r="G242" t="n">
+      <c r="G247" t="n">
         <v>2004</v>
       </c>
-      <c r="H242" t="inlineStr">
+      <c r="H247" t="inlineStr">
         <is>
           <t>conf/icsm/2004</t>
         </is>
       </c>
     </row>
-    <row r="243">
-      <c r="A243" t="inlineStr">
+    <row r="248">
+      <c r="A248" t="inlineStr">
         <is>
           <t>Audris Mockus and Lawrence G. Votta</t>
         </is>
       </c>
-      <c r="B243" t="inlineStr">
+      <c r="B248" t="inlineStr">
         <is>
           <t>@inproceedings{mockus:2000,
 booktitle = {International Conference on Software Maintenance and Evolution (ICSME)}, 
@@ -10693,42 +10918,42 @@
 }</t>
         </is>
       </c>
-      <c r="C243" t="inlineStr">
+      <c r="C248" t="inlineStr">
         <is>
           <t>conf/icsm/MockusV00</t>
         </is>
       </c>
-      <c r="D243" t="inlineStr">
+      <c r="D248" t="inlineStr">
         <is>
           <t>Identifying Reasons for Software Changes using Historic Databases</t>
         </is>
       </c>
-      <c r="E243" t="inlineStr">
+      <c r="E248" t="inlineStr">
         <is>
           <t>db/conf/icsm/icsm2000.html#MockusV00</t>
         </is>
       </c>
-      <c r="F243" t="inlineStr">
+      <c r="F248" t="inlineStr">
         <is>
           <t>conf/icsm/</t>
         </is>
       </c>
-      <c r="G243" t="n">
+      <c r="G248" t="n">
         <v>2000</v>
       </c>
-      <c r="H243" t="inlineStr">
+      <c r="H248" t="inlineStr">
         <is>
           <t>conf/icsm/2000</t>
         </is>
       </c>
     </row>
-    <row r="244">
-      <c r="A244" t="inlineStr">
+    <row r="249">
+      <c r="A249" t="inlineStr">
         <is>
           <t>Yingjun Lyu and Jiaping Gui and Mian Wan and William G. J. Halfond</t>
         </is>
       </c>
-      <c r="B244" t="inlineStr">
+      <c r="B249" t="inlineStr">
         <is>
           <t>@inproceedings{lyu:2017,
 booktitle = {International Conference on Software Maintenance and Evolution (ICSME)}, 
@@ -10738,42 +10963,42 @@
 }</t>
         </is>
       </c>
-      <c r="C244" t="inlineStr">
+      <c r="C249" t="inlineStr">
         <is>
           <t>conf/icsm/LyuGWH17</t>
         </is>
       </c>
-      <c r="D244" t="inlineStr">
+      <c r="D249" t="inlineStr">
         <is>
           <t>An Empirical Study of Local Database Usage in Android Applications</t>
         </is>
       </c>
-      <c r="E244" t="inlineStr">
+      <c r="E249" t="inlineStr">
         <is>
           <t>db/conf/icsm/icsme2017.html#LyuGWH17</t>
         </is>
       </c>
-      <c r="F244" t="inlineStr">
+      <c r="F249" t="inlineStr">
         <is>
           <t>conf/icsm/</t>
         </is>
       </c>
-      <c r="G244" t="n">
+      <c r="G249" t="n">
         <v>2017</v>
       </c>
-      <c r="H244" t="inlineStr">
+      <c r="H249" t="inlineStr">
         <is>
           <t>conf/icsm/2017</t>
         </is>
       </c>
     </row>
-    <row r="245">
-      <c r="A245" t="inlineStr">
+    <row r="250">
+      <c r="A250" t="inlineStr">
         <is>
           <t>Véronique Narat</t>
         </is>
       </c>
-      <c r="B245" t="inlineStr">
+      <c r="B250" t="inlineStr">
         <is>
           <t>@inproceedings{narat:1993,
 booktitle = {International Conference on Software Maintenance and Evolution (ICSME)}, 
@@ -10783,42 +11008,42 @@
 }</t>
         </is>
       </c>
-      <c r="C245" t="inlineStr">
+      <c r="C250" t="inlineStr">
         <is>
           <t>conf/icsm/Narat93</t>
         </is>
       </c>
-      <c r="D245" t="inlineStr">
+      <c r="D250" t="inlineStr">
         <is>
           <t>Using a Relational Database for Software Maintenance: A Case Study</t>
         </is>
       </c>
-      <c r="E245" t="inlineStr">
+      <c r="E250" t="inlineStr">
         <is>
           <t>db/conf/icsm/icsm1993.html#Narat93</t>
         </is>
       </c>
-      <c r="F245" t="inlineStr">
+      <c r="F250" t="inlineStr">
         <is>
           <t>conf/icsm/</t>
         </is>
       </c>
-      <c r="G245" t="n">
+      <c r="G250" t="n">
         <v>1993</v>
       </c>
-      <c r="H245" t="inlineStr">
+      <c r="H250" t="inlineStr">
         <is>
           <t>conf/icsm/1993</t>
         </is>
       </c>
     </row>
-    <row r="246">
-      <c r="A246" t="inlineStr">
+    <row r="251">
+      <c r="A251" t="inlineStr">
         <is>
           <t>Stefan Strobl and Mario Bernhart and Thomas Grechenig and Wolfgang Kleinert</t>
         </is>
       </c>
-      <c r="B246" t="inlineStr">
+      <c r="B251" t="inlineStr">
         <is>
           <t>@inproceedings{strobl:2009,
 booktitle = {International Conference on Software Maintenance and Evolution (ICSME)}, 
@@ -10828,42 +11053,42 @@
 }</t>
         </is>
       </c>
-      <c r="C246" t="inlineStr">
+      <c r="C251" t="inlineStr">
         <is>
           <t>conf/icsm/StroblBGK09</t>
         </is>
       </c>
-      <c r="D246" t="inlineStr">
+      <c r="D251" t="inlineStr">
         <is>
           <t>Digging deep: Software reengineering supported by database reverse engineering of a system with 30+ years of legacy</t>
         </is>
       </c>
-      <c r="E246" t="inlineStr">
+      <c r="E251" t="inlineStr">
         <is>
           <t>db/conf/icsm/icsm2009.html#StroblBGK09</t>
         </is>
       </c>
-      <c r="F246" t="inlineStr">
+      <c r="F251" t="inlineStr">
         <is>
           <t>conf/icsm/</t>
         </is>
       </c>
-      <c r="G246" t="n">
+      <c r="G251" t="n">
         <v>2009</v>
       </c>
-      <c r="H246" t="inlineStr">
+      <c r="H251" t="inlineStr">
         <is>
           <t>conf/icsm/2009</t>
         </is>
       </c>
     </row>
-    <row r="247">
-      <c r="A247" t="inlineStr">
+    <row r="252">
+      <c r="A252" t="inlineStr">
         <is>
           <t>Phil McMinn and Chris J. Wright and Cody Kinneer and Colton J. McCurdy and Michael Camara and Gregory M. Kapfhammer</t>
         </is>
       </c>
-      <c r="B247" t="inlineStr">
+      <c r="B252" t="inlineStr">
         <is>
           <t>@inproceedings{mcminn:2016,
 booktitle = {International Conference on Software Maintenance and Evolution (ICSME)}, 
@@ -10873,42 +11098,42 @@
 }</t>
         </is>
       </c>
-      <c r="C247" t="inlineStr">
+      <c r="C252" t="inlineStr">
         <is>
           <t>conf/icsm/McMinnWKMCK16</t>
         </is>
       </c>
-      <c r="D247" t="inlineStr">
+      <c r="D252" t="inlineStr">
         <is>
           <t>SchemaAnalyst: Search-Based Test Data Generation for Relational Database Schemas</t>
         </is>
       </c>
-      <c r="E247" t="inlineStr">
+      <c r="E252" t="inlineStr">
         <is>
           <t>db/conf/icsm/icsme2016.html#McMinnWKMCK16</t>
         </is>
       </c>
-      <c r="F247" t="inlineStr">
+      <c r="F252" t="inlineStr">
         <is>
           <t>conf/icsm/</t>
         </is>
       </c>
-      <c r="G247" t="n">
+      <c r="G252" t="n">
         <v>2016</v>
       </c>
-      <c r="H247" t="inlineStr">
+      <c r="H252" t="inlineStr">
         <is>
           <t>conf/icsm/2016</t>
         </is>
       </c>
     </row>
-    <row r="248">
-      <c r="A248" t="inlineStr">
+    <row r="253">
+      <c r="A253" t="inlineStr">
         <is>
           <t>Laurent Deruelle and Mourad Bouneffa and Nordine Melab and Henri Basson</t>
         </is>
       </c>
-      <c r="B248" t="inlineStr">
+      <c r="B253" t="inlineStr">
         <is>
           <t>@inproceedings{deruelle:2001,
 booktitle = {International Conference on Software Maintenance and Evolution (ICSME)}, 
@@ -10918,42 +11143,42 @@
 }</t>
         </is>
       </c>
-      <c r="C248" t="inlineStr">
+      <c r="C253" t="inlineStr">
         <is>
           <t>conf/icsm/DeruelleBMB01</t>
         </is>
       </c>
-      <c r="D248" t="inlineStr">
+      <c r="D253" t="inlineStr">
         <is>
           <t>A Change Propagation Model and Platform for Multi-Database Applications</t>
         </is>
       </c>
-      <c r="E248" t="inlineStr">
+      <c r="E253" t="inlineStr">
         <is>
           <t>db/conf/icsm/icsm2001.html#DeruelleBMB01</t>
         </is>
       </c>
-      <c r="F248" t="inlineStr">
+      <c r="F253" t="inlineStr">
         <is>
           <t>conf/icsm/</t>
         </is>
       </c>
-      <c r="G248" t="n">
+      <c r="G253" t="n">
         <v>2001</v>
       </c>
-      <c r="H248" t="inlineStr">
+      <c r="H253" t="inlineStr">
         <is>
           <t>conf/icsm/2001</t>
         </is>
       </c>
     </row>
-    <row r="249">
-      <c r="A249" t="inlineStr">
+    <row r="254">
+      <c r="A254" t="inlineStr">
         <is>
           <t>Erik Rogstad and Lionel C. Briand and Ronny Dalberg and Marianne Rynning and Erik Arisholm</t>
         </is>
       </c>
-      <c r="B249" t="inlineStr">
+      <c r="B254" t="inlineStr">
         <is>
           <t>@inproceedings{rogstad:2011,
 booktitle = {International Conference on Software Maintenance and Evolution (ICSME)}, 
@@ -10963,42 +11188,42 @@
 }</t>
         </is>
       </c>
-      <c r="C249" t="inlineStr">
+      <c r="C254" t="inlineStr">
         <is>
           <t>conf/icsm/RogstadBDRA11</t>
         </is>
       </c>
-      <c r="D249" t="inlineStr">
+      <c r="D254" t="inlineStr">
         <is>
           <t>Industrial experiences with automated regression testing of a legacy database application</t>
         </is>
       </c>
-      <c r="E249" t="inlineStr">
+      <c r="E254" t="inlineStr">
         <is>
           <t>db/conf/icsm/icsm2011.html#RogstadBDRA11</t>
         </is>
       </c>
-      <c r="F249" t="inlineStr">
+      <c r="F254" t="inlineStr">
         <is>
           <t>conf/icsm/</t>
         </is>
       </c>
-      <c r="G249" t="n">
+      <c r="G254" t="n">
         <v>2011</v>
       </c>
-      <c r="H249" t="inlineStr">
+      <c r="H254" t="inlineStr">
         <is>
           <t>conf/icsm/2011</t>
         </is>
       </c>
     </row>
-    <row r="250">
-      <c r="A250" t="inlineStr">
+    <row r="255">
+      <c r="A255" t="inlineStr">
         <is>
           <t>Donatella Castelli</t>
         </is>
       </c>
-      <c r="B250" t="inlineStr">
+      <c r="B255" t="inlineStr">
         <is>
           <t>@inproceedings{castelli:1998,
 booktitle = {International Conference on Software Maintenance and Evolution (ICSME)}, 
@@ -11008,42 +11233,42 @@
 }</t>
         </is>
       </c>
-      <c r="C250" t="inlineStr">
+      <c r="C255" t="inlineStr">
         <is>
           <t>conf/icsm/Castelli98</t>
         </is>
       </c>
-      <c r="D250" t="inlineStr">
+      <c r="D255" t="inlineStr">
         <is>
           <t>Reuse in Replaying Database Design</t>
         </is>
       </c>
-      <c r="E250" t="inlineStr">
+      <c r="E255" t="inlineStr">
         <is>
           <t>db/conf/icsm/icsm1998.html#Castelli98</t>
         </is>
       </c>
-      <c r="F250" t="inlineStr">
+      <c r="F255" t="inlineStr">
         <is>
           <t>conf/icsm/</t>
         </is>
       </c>
-      <c r="G250" t="n">
+      <c r="G255" t="n">
         <v>1998</v>
       </c>
-      <c r="H250" t="inlineStr">
+      <c r="H255" t="inlineStr">
         <is>
           <t>conf/icsm/1998</t>
         </is>
       </c>
     </row>
-    <row r="251">
-      <c r="A251" t="inlineStr">
+    <row r="256">
+      <c r="A256" t="inlineStr">
         <is>
           <t>Maxime Gobert and Jerome Maes and Anthony Cleve and Jens H. Weber</t>
         </is>
       </c>
-      <c r="B251" t="inlineStr">
+      <c r="B256" t="inlineStr">
         <is>
           <t>@inproceedings{gobert:2013,
 booktitle = {International Conference on Software Maintenance and Evolution (ICSME)}, 
@@ -11053,42 +11278,42 @@
 }</t>
         </is>
       </c>
-      <c r="C251" t="inlineStr">
+      <c r="C256" t="inlineStr">
         <is>
           <t>conf/icsm/GobertMCW13</t>
         </is>
       </c>
-      <c r="D251" t="inlineStr">
+      <c r="D256" t="inlineStr">
         <is>
           <t>Understanding Schema Evolution as a Basis for Database Reengineering</t>
         </is>
       </c>
-      <c r="E251" t="inlineStr">
+      <c r="E256" t="inlineStr">
         <is>
           <t>db/conf/icsm/icsm2013.html#GobertMCW13</t>
         </is>
       </c>
-      <c r="F251" t="inlineStr">
+      <c r="F256" t="inlineStr">
         <is>
           <t>conf/icsm/</t>
         </is>
       </c>
-      <c r="G251" t="n">
+      <c r="G256" t="n">
         <v>2013</v>
       </c>
-      <c r="H251" t="inlineStr">
+      <c r="H256" t="inlineStr">
         <is>
           <t>conf/icsm/2013</t>
         </is>
       </c>
     </row>
-    <row r="252">
-      <c r="A252" t="inlineStr">
+    <row r="257">
+      <c r="A257" t="inlineStr">
         <is>
           <t>Abram Hindle and Michael W. Godfrey and Richard C. Holt</t>
         </is>
       </c>
-      <c r="B252" t="inlineStr">
+      <c r="B257" t="inlineStr">
         <is>
           <t>@inproceedings{hindle:2007,
 booktitle = {International Conference on Software Maintenance and Evolution (ICSME)}, 
@@ -11098,42 +11323,42 @@
 }</t>
         </is>
       </c>
-      <c r="C252" t="inlineStr">
+      <c r="C257" t="inlineStr">
         <is>
           <t>conf/icsm/HindleGH07</t>
         </is>
       </c>
-      <c r="D252" t="inlineStr">
+      <c r="D257" t="inlineStr">
         <is>
           <t>Release Pattern Discovery: A Case Study of Database Systems</t>
         </is>
       </c>
-      <c r="E252" t="inlineStr">
+      <c r="E257" t="inlineStr">
         <is>
           <t>db/conf/icsm/icsm2007.html#HindleGH07</t>
         </is>
       </c>
-      <c r="F252" t="inlineStr">
+      <c r="F257" t="inlineStr">
         <is>
           <t>conf/icsm/</t>
         </is>
       </c>
-      <c r="G252" t="n">
+      <c r="G257" t="n">
         <v>2007</v>
       </c>
-      <c r="H252" t="inlineStr">
+      <c r="H257" t="inlineStr">
         <is>
           <t>conf/icsm/2007</t>
         </is>
       </c>
     </row>
-    <row r="253">
-      <c r="A253" t="inlineStr">
+    <row r="258">
+      <c r="A258" t="inlineStr">
         <is>
           <t>Awais Rashid</t>
         </is>
       </c>
-      <c r="B253" t="inlineStr">
+      <c r="B258" t="inlineStr">
         <is>
           <t>@inproceedings{rashid:2001,
 booktitle = {International Conference on Software Maintenance and Evolution (ICSME)}, 
@@ -11143,42 +11368,42 @@
 }</t>
         </is>
       </c>
-      <c r="C253" t="inlineStr">
+      <c r="C258" t="inlineStr">
         <is>
           <t>conf/icsm/Rashid01</t>
         </is>
       </c>
-      <c r="D253" t="inlineStr">
+      <c r="D258" t="inlineStr">
         <is>
           <t>A Database Evolution Approach for Object-Oriented Databases</t>
         </is>
       </c>
-      <c r="E253" t="inlineStr">
+      <c r="E258" t="inlineStr">
         <is>
           <t>db/conf/icsm/icsm2001.html#Rashid01</t>
         </is>
       </c>
-      <c r="F253" t="inlineStr">
+      <c r="F258" t="inlineStr">
         <is>
           <t>conf/icsm/</t>
         </is>
       </c>
-      <c r="G253" t="n">
+      <c r="G258" t="n">
         <v>2001</v>
       </c>
-      <c r="H253" t="inlineStr">
+      <c r="H258" t="inlineStr">
         <is>
           <t>conf/icsm/2001</t>
         </is>
       </c>
     </row>
-    <row r="254">
-      <c r="A254" t="inlineStr">
+    <row r="259">
+      <c r="A259" t="inlineStr">
         <is>
           <t>Hung Viet Nguyen and Hoan Anh Nguyen and Tung Thanh Nguyen and Tien N. Nguyen</t>
         </is>
       </c>
-      <c r="B254" t="inlineStr">
+      <c r="B259" t="inlineStr">
         <is>
           <t>@inproceedings{viet:2013,
 booktitle = {International Conference on Software Maintenance and Evolution (ICSME)}, 
@@ -11188,42 +11413,42 @@
 }</t>
         </is>
       </c>
-      <c r="C254" t="inlineStr">
+      <c r="C259" t="inlineStr">
         <is>
           <t>conf/icsm/NguyenNNN13a</t>
         </is>
       </c>
-      <c r="D254" t="inlineStr">
+      <c r="D259" t="inlineStr">
         <is>
           <t>Database-Aware Fault Localization for Dynamic Web Applications</t>
         </is>
       </c>
-      <c r="E254" t="inlineStr">
+      <c r="E259" t="inlineStr">
         <is>
           <t>db/conf/icsm/icsm2013.html#NguyenNNN13a</t>
         </is>
       </c>
-      <c r="F254" t="inlineStr">
+      <c r="F259" t="inlineStr">
         <is>
           <t>conf/icsm/</t>
         </is>
       </c>
-      <c r="G254" t="n">
+      <c r="G259" t="n">
         <v>2013</v>
       </c>
-      <c r="H254" t="inlineStr">
+      <c r="H259" t="inlineStr">
         <is>
           <t>conf/icsm/2013</t>
         </is>
       </c>
     </row>
-    <row r="255">
-      <c r="A255" t="inlineStr">
+    <row r="260">
+      <c r="A260" t="inlineStr">
         <is>
           <t>Michael Fischer 0001 and Martin Pinzger 0001 and Harald C. Gall</t>
         </is>
       </c>
-      <c r="B255" t="inlineStr">
+      <c r="B260" t="inlineStr">
         <is>
           <t>@inproceedings{fischer:2003,
 booktitle = {International Conference on Software Maintenance and Evolution (ICSME)}, 
@@ -11233,42 +11458,42 @@
 }</t>
         </is>
       </c>
-      <c r="C255" t="inlineStr">
+      <c r="C260" t="inlineStr">
         <is>
           <t>conf/icsm/FischerPG03</t>
         </is>
       </c>
-      <c r="D255" t="inlineStr">
+      <c r="D260" t="inlineStr">
         <is>
           <t>Populating a Release History Database from Version Control and Bug Tracking Systems</t>
         </is>
       </c>
-      <c r="E255" t="inlineStr">
+      <c r="E260" t="inlineStr">
         <is>
           <t>db/conf/icsm/icsm2003.html#FischerPG03</t>
         </is>
       </c>
-      <c r="F255" t="inlineStr">
+      <c r="F260" t="inlineStr">
         <is>
           <t>conf/icsm/</t>
         </is>
       </c>
-      <c r="G255" t="n">
+      <c r="G260" t="n">
         <v>2003</v>
       </c>
-      <c r="H255" t="inlineStr">
+      <c r="H260" t="inlineStr">
         <is>
           <t>conf/icsm/2003</t>
         </is>
       </c>
     </row>
-    <row r="256">
-      <c r="A256" t="inlineStr">
+    <row r="261">
+      <c r="A261" t="inlineStr">
         <is>
           <t>David Willmor and Suzanne M. Embury</t>
         </is>
       </c>
-      <c r="B256" t="inlineStr">
+      <c r="B261" t="inlineStr">
         <is>
           <t>@inproceedings{willmor:2005,
 booktitle = {International Conference on Software Maintenance and Evolution (ICSME)}, 
@@ -11278,30 +11503,30 @@
 }</t>
         </is>
       </c>
-      <c r="C256" t="inlineStr">
+      <c r="C261" t="inlineStr">
         <is>
           <t>conf/icsm/WillmorE05</t>
         </is>
       </c>
-      <c r="D256" t="inlineStr">
+      <c r="D261" t="inlineStr">
         <is>
           <t>A Safe Regression Test Selection Technique for Database-Driven Applications</t>
         </is>
       </c>
-      <c r="E256" t="inlineStr">
+      <c r="E261" t="inlineStr">
         <is>
           <t>db/conf/icsm/icsm2005.html#WillmorE05</t>
         </is>
       </c>
-      <c r="F256" t="inlineStr">
+      <c r="F261" t="inlineStr">
         <is>
           <t>conf/icsm/</t>
         </is>
       </c>
-      <c r="G256" t="n">
+      <c r="G261" t="n">
         <v>2005</v>
       </c>
-      <c r="H256" t="inlineStr">
+      <c r="H261" t="inlineStr">
         <is>
           <t>conf/icsm/2005</t>
         </is>

</xml_diff>